<commit_message>
Loging page is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/gigatron.xlsx
+++ b/src/test/test_data/gigatron.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\iponhu\src\test\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\gigatron\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549D9F04-D79E-4683-98C8-5B7EE622B8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B456F263-B252-479F-A2F8-2A53B8469770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="140">
   <si>
     <t>tc_id</t>
   </si>
@@ -436,13 +436,25 @@
   </si>
   <si>
     <t>3300 Eger, Hajduk Veljkova</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Kikinda@06</t>
+  </si>
+  <si>
+    <t>urlMessage</t>
+  </si>
+  <si>
+    <t>https://gigatron.rs/korisnik</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,6 +499,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -572,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -602,6 +644,9 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -620,8 +665,28 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -944,195 +1009,193 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D05107-472F-4DD1-88F8-DE97CAF36E00}">
   <dimension ref="A1:AJ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="20" style="1" customWidth="1"/>
-    <col min="15" max="16" width="17.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="24" style="1" customWidth="1"/>
-    <col min="18" max="18" width="21.5703125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="5.7109375" style="1" customWidth="1"/>
-    <col min="23" max="23" width="8" style="1" customWidth="1"/>
-    <col min="24" max="24" width="13" style="1" customWidth="1"/>
-    <col min="25" max="25" width="10.7109375" style="1" customWidth="1"/>
-    <col min="26" max="26" width="23.28515625" style="1" customWidth="1"/>
-    <col min="27" max="28" width="16.7109375" style="1" customWidth="1"/>
-    <col min="29" max="29" width="17.140625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="16.140625" style="1" customWidth="1"/>
-    <col min="32" max="32" width="21.140625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="30.85546875" style="1" customWidth="1"/>
-    <col min="34" max="34" width="17" style="1" customWidth="1"/>
-    <col min="35" max="35" width="15.7109375" style="1" customWidth="1"/>
-    <col min="36" max="36" width="14.42578125" style="1" customWidth="1"/>
-    <col min="37" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8.140625" style="30" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="22" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="22" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="20" style="22" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="22" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="22" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="22" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="22" customWidth="1"/>
+    <col min="14" max="14" width="20" style="22" customWidth="1"/>
+    <col min="15" max="16" width="17.42578125" style="22" customWidth="1"/>
+    <col min="17" max="17" width="24" style="22" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" style="22" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" style="22" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" style="22" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" style="22" customWidth="1"/>
+    <col min="22" max="22" width="5.7109375" style="22" customWidth="1"/>
+    <col min="23" max="23" width="8" style="22" customWidth="1"/>
+    <col min="24" max="24" width="13" style="22" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" style="22" customWidth="1"/>
+    <col min="26" max="26" width="23.28515625" style="22" customWidth="1"/>
+    <col min="27" max="28" width="16.7109375" style="22" customWidth="1"/>
+    <col min="29" max="29" width="17.140625" style="22" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="22" customWidth="1"/>
+    <col min="31" max="31" width="16.140625" style="22" customWidth="1"/>
+    <col min="32" max="32" width="21.140625" style="22" customWidth="1"/>
+    <col min="33" max="33" width="30.85546875" style="22" customWidth="1"/>
+    <col min="34" max="34" width="17" style="22" customWidth="1"/>
+    <col min="35" max="35" width="15.7109375" style="22" customWidth="1"/>
+    <col min="36" max="36" width="14.42578125" style="22" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="14"/>
-      <c r="AG1" s="14"/>
-      <c r="AH1" s="14"/>
-      <c r="AI1" s="14"/>
-      <c r="AJ1" s="14"/>
-    </row>
-    <row r="2" spans="1:36" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-    </row>
-    <row r="3" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="21"/>
+      <c r="AE1" s="21"/>
+      <c r="AF1" s="21"/>
+      <c r="AG1" s="21"/>
+      <c r="AH1" s="21"/>
+      <c r="AI1" s="21"/>
+      <c r="AJ1" s="21"/>
+    </row>
+    <row r="2" spans="1:36" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23"/>
+    </row>
+    <row r="3" spans="1:36" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U3" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="X3" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="Y3" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="Z3" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="6"/>
-      <c r="AH3" s="6"/>
-      <c r="AI3" s="6"/>
-      <c r="AJ3" s="6"/>
-    </row>
-    <row r="4" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24"/>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="24"/>
+      <c r="AH3" s="24"/>
+      <c r="AI3" s="24"/>
+      <c r="AJ3" s="24"/>
+    </row>
+    <row r="4" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
-        <v>30</v>
+      <c r="B4" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>137</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -1202,21 +1265,17 @@
       <c r="AI4" s="7"/>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>31</v>
+      <c r="E5" s="27" t="s">
+        <v>137</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -1233,7 +1292,7 @@
       <c r="L5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="M5" s="5"/>
+      <c r="M5" s="28"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
@@ -1258,21 +1317,17 @@
       <c r="AI5" s="7"/>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>30</v>
+      <c r="E6" s="27" t="s">
+        <v>137</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>34</v>
@@ -1287,7 +1342,7 @@
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
-      <c r="M6" s="5"/>
+      <c r="M6" s="28"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -1312,21 +1367,17 @@
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>31</v>
+      <c r="E7" s="27" t="s">
+        <v>137</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>34</v>
@@ -1341,7 +1392,7 @@
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="5"/>
+      <c r="M7" s="28"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
@@ -1366,19 +1417,17 @@
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="7"/>
-      <c r="C8" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>30</v>
+      <c r="E8" s="27" t="s">
+        <v>137</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>34</v>
@@ -1393,14 +1442,14 @@
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="5"/>
+      <c r="M8" s="28"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
@@ -1418,19 +1467,15 @@
       <c r="AI8" s="7"/>
       <c r="AJ8" s="7"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="7" t="s">
-        <v>31</v>
+      <c r="E9" s="27" t="s">
+        <v>137</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>34</v>
@@ -1445,7 +1490,7 @@
       </c>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="5"/>
+      <c r="M9" s="28"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
@@ -1470,8 +1515,8 @@
       <c r="AI9" s="7"/>
       <c r="AJ9" s="7"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="7"/>
@@ -1510,8 +1555,8 @@
       <c r="AI10" s="7"/>
       <c r="AJ10" s="7"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A11" s="26" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="7"/>
@@ -1525,33 +1570,33 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
-      <c r="M11" s="5"/>
+      <c r="M11" s="28"/>
       <c r="N11" s="7"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
-      <c r="AA11" s="5"/>
-      <c r="AB11" s="5"/>
-      <c r="AC11" s="5"/>
-      <c r="AD11" s="5"/>
-      <c r="AE11" s="5"/>
-      <c r="AF11" s="5"/>
-      <c r="AG11" s="5"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="28"/>
+      <c r="T11" s="28"/>
+      <c r="U11" s="28"/>
+      <c r="V11" s="28"/>
+      <c r="W11" s="28"/>
+      <c r="X11" s="28"/>
+      <c r="Y11" s="28"/>
+      <c r="Z11" s="28"/>
+      <c r="AA11" s="28"/>
+      <c r="AB11" s="28"/>
+      <c r="AC11" s="28"/>
+      <c r="AD11" s="28"/>
+      <c r="AE11" s="28"/>
+      <c r="AF11" s="28"/>
+      <c r="AG11" s="28"/>
       <c r="AH11" s="7"/>
       <c r="AI11" s="7"/>
       <c r="AJ11" s="7"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A12" s="26" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="7"/>
@@ -1564,38 +1609,40 @@
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="5"/>
-      <c r="Y12" s="5"/>
-      <c r="Z12" s="5"/>
-      <c r="AA12" s="5"/>
-      <c r="AB12" s="5"/>
-      <c r="AC12" s="5"/>
-      <c r="AD12" s="5"/>
-      <c r="AE12" s="5"/>
-      <c r="AF12" s="5"/>
-      <c r="AG12" s="5"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="28"/>
+      <c r="U12" s="28"/>
+      <c r="V12" s="28"/>
+      <c r="W12" s="28"/>
+      <c r="X12" s="28"/>
+      <c r="Y12" s="28"/>
+      <c r="Z12" s="28"/>
+      <c r="AA12" s="28"/>
+      <c r="AB12" s="28"/>
+      <c r="AC12" s="28"/>
+      <c r="AD12" s="28"/>
+      <c r="AE12" s="28"/>
+      <c r="AF12" s="28"/>
+      <c r="AG12" s="28"/>
       <c r="AH12" s="7"/>
       <c r="AI12" s="7"/>
       <c r="AJ12" s="7"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="C13" s="7" t="s">
+        <v>136</v>
+      </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -1604,34 +1651,34 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
-      <c r="X13" s="5"/>
-      <c r="Y13" s="5"/>
-      <c r="Z13" s="5"/>
-      <c r="AA13" s="5"/>
-      <c r="AB13" s="5"/>
-      <c r="AC13" s="5"/>
-      <c r="AD13" s="5"/>
-      <c r="AE13" s="5"/>
-      <c r="AF13" s="5"/>
-      <c r="AG13" s="5"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="28"/>
+      <c r="X13" s="28"/>
+      <c r="Y13" s="28"/>
+      <c r="Z13" s="28"/>
+      <c r="AA13" s="28"/>
+      <c r="AB13" s="28"/>
+      <c r="AC13" s="28"/>
+      <c r="AD13" s="28"/>
+      <c r="AE13" s="28"/>
+      <c r="AF13" s="28"/>
+      <c r="AG13" s="28"/>
       <c r="AH13" s="7"/>
       <c r="AI13" s="7"/>
       <c r="AJ13" s="7"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A14" s="26" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="7"/>
@@ -1644,34 +1691,34 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="5"/>
-      <c r="W14" s="5"/>
-      <c r="X14" s="5"/>
-      <c r="Y14" s="5"/>
-      <c r="Z14" s="5"/>
-      <c r="AA14" s="5"/>
-      <c r="AB14" s="5"/>
-      <c r="AC14" s="5"/>
-      <c r="AD14" s="5"/>
-      <c r="AE14" s="5"/>
-      <c r="AF14" s="5"/>
-      <c r="AG14" s="5"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
+      <c r="W14" s="28"/>
+      <c r="X14" s="28"/>
+      <c r="Y14" s="28"/>
+      <c r="Z14" s="28"/>
+      <c r="AA14" s="28"/>
+      <c r="AB14" s="28"/>
+      <c r="AC14" s="28"/>
+      <c r="AD14" s="28"/>
+      <c r="AE14" s="28"/>
+      <c r="AF14" s="28"/>
+      <c r="AG14" s="28"/>
       <c r="AH14" s="7"/>
       <c r="AI14" s="7"/>
       <c r="AJ14" s="7"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A15" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="7"/>
@@ -1684,34 +1731,34 @@
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="5"/>
-      <c r="Z15" s="5"/>
-      <c r="AA15" s="5"/>
-      <c r="AB15" s="5"/>
-      <c r="AC15" s="5"/>
-      <c r="AD15" s="5"/>
-      <c r="AE15" s="5"/>
-      <c r="AF15" s="5"/>
-      <c r="AG15" s="5"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="28"/>
+      <c r="Z15" s="28"/>
+      <c r="AA15" s="28"/>
+      <c r="AB15" s="28"/>
+      <c r="AC15" s="28"/>
+      <c r="AD15" s="28"/>
+      <c r="AE15" s="28"/>
+      <c r="AF15" s="28"/>
+      <c r="AG15" s="28"/>
       <c r="AH15" s="7"/>
       <c r="AI15" s="7"/>
       <c r="AJ15" s="7"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A16" s="26" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="7"/>
@@ -1724,34 +1771,34 @@
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="5"/>
-      <c r="W16" s="9"/>
-      <c r="X16" s="9"/>
-      <c r="Y16" s="9"/>
-      <c r="Z16" s="9"/>
-      <c r="AA16" s="9"/>
-      <c r="AB16" s="9"/>
-      <c r="AC16" s="9"/>
-      <c r="AD16" s="9"/>
-      <c r="AE16" s="9"/>
-      <c r="AF16" s="9"/>
-      <c r="AG16" s="9"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="29"/>
+      <c r="X16" s="29"/>
+      <c r="Y16" s="29"/>
+      <c r="Z16" s="29"/>
+      <c r="AA16" s="29"/>
+      <c r="AB16" s="29"/>
+      <c r="AC16" s="29"/>
+      <c r="AD16" s="29"/>
+      <c r="AE16" s="29"/>
+      <c r="AF16" s="29"/>
+      <c r="AG16" s="29"/>
       <c r="AH16" s="8"/>
       <c r="AI16" s="7"/>
       <c r="AJ16" s="7"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A17" s="26" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="7"/>
@@ -1764,114 +1811,114 @@
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5"/>
-      <c r="X17" s="5"/>
-      <c r="Y17" s="5"/>
-      <c r="Z17" s="5"/>
-      <c r="AA17" s="5"/>
-      <c r="AB17" s="5"/>
-      <c r="AC17" s="5"/>
-      <c r="AD17" s="5"/>
-      <c r="AE17" s="5"/>
-      <c r="AF17" s="5"/>
-      <c r="AG17" s="5"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="28"/>
+      <c r="S17" s="28"/>
+      <c r="T17" s="28"/>
+      <c r="U17" s="28"/>
+      <c r="V17" s="28"/>
+      <c r="W17" s="28"/>
+      <c r="X17" s="28"/>
+      <c r="Y17" s="28"/>
+      <c r="Z17" s="28"/>
+      <c r="AA17" s="28"/>
+      <c r="AB17" s="28"/>
+      <c r="AC17" s="28"/>
+      <c r="AD17" s="28"/>
+      <c r="AE17" s="28"/>
+      <c r="AF17" s="28"/>
+      <c r="AG17" s="28"/>
       <c r="AH17" s="7"/>
       <c r="AI17" s="7"/>
       <c r="AJ17" s="7"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A18" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
-      <c r="V18" s="5"/>
-      <c r="W18" s="5"/>
-      <c r="X18" s="5"/>
-      <c r="Y18" s="5"/>
-      <c r="Z18" s="5"/>
-      <c r="AA18" s="5"/>
-      <c r="AB18" s="5"/>
-      <c r="AC18" s="5"/>
-      <c r="AD18" s="5"/>
-      <c r="AE18" s="5"/>
-      <c r="AF18" s="5"/>
-      <c r="AG18" s="5"/>
-      <c r="AH18" s="5"/>
-      <c r="AI18" s="5"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="28"/>
+      <c r="U18" s="28"/>
+      <c r="V18" s="28"/>
+      <c r="W18" s="28"/>
+      <c r="X18" s="28"/>
+      <c r="Y18" s="28"/>
+      <c r="Z18" s="28"/>
+      <c r="AA18" s="28"/>
+      <c r="AB18" s="28"/>
+      <c r="AC18" s="28"/>
+      <c r="AD18" s="28"/>
+      <c r="AE18" s="28"/>
+      <c r="AF18" s="28"/>
+      <c r="AG18" s="28"/>
+      <c r="AH18" s="28"/>
+      <c r="AI18" s="28"/>
       <c r="AJ18" s="7"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A19" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
-      <c r="V19" s="5"/>
-      <c r="W19" s="5"/>
-      <c r="X19" s="5"/>
-      <c r="Y19" s="5"/>
-      <c r="Z19" s="5"/>
-      <c r="AA19" s="5"/>
-      <c r="AB19" s="5"/>
-      <c r="AC19" s="5"/>
-      <c r="AD19" s="5"/>
-      <c r="AE19" s="5"/>
-      <c r="AF19" s="5"/>
-      <c r="AG19" s="5"/>
-      <c r="AH19" s="5"/>
-      <c r="AI19" s="5"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="28"/>
+      <c r="S19" s="28"/>
+      <c r="T19" s="28"/>
+      <c r="U19" s="28"/>
+      <c r="V19" s="28"/>
+      <c r="W19" s="28"/>
+      <c r="X19" s="28"/>
+      <c r="Y19" s="28"/>
+      <c r="Z19" s="28"/>
+      <c r="AA19" s="28"/>
+      <c r="AB19" s="28"/>
+      <c r="AC19" s="28"/>
+      <c r="AD19" s="28"/>
+      <c r="AE19" s="28"/>
+      <c r="AF19" s="28"/>
+      <c r="AG19" s="28"/>
+      <c r="AH19" s="28"/>
+      <c r="AI19" s="28"/>
       <c r="AJ19" s="7"/>
     </row>
-    <row r="20" spans="1:36" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:36" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="7"/>
@@ -1910,8 +1957,8 @@
       <c r="AI20" s="7"/>
       <c r="AJ20" s="7"/>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A21" s="26"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1922,28 +1969,28 @@
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="9"/>
-      <c r="Y21" s="9"/>
-      <c r="Z21" s="9"/>
-      <c r="AA21" s="9"/>
-      <c r="AB21" s="9"/>
-      <c r="AC21" s="9"/>
-      <c r="AD21" s="9"/>
-      <c r="AE21" s="9"/>
-      <c r="AF21" s="9"/>
-      <c r="AG21" s="9"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
+      <c r="U21" s="29"/>
+      <c r="V21" s="29"/>
+      <c r="W21" s="29"/>
+      <c r="X21" s="29"/>
+      <c r="Y21" s="29"/>
+      <c r="Z21" s="29"/>
+      <c r="AA21" s="29"/>
+      <c r="AB21" s="29"/>
+      <c r="AC21" s="29"/>
+      <c r="AD21" s="29"/>
+      <c r="AE21" s="29"/>
+      <c r="AF21" s="29"/>
+      <c r="AG21" s="29"/>
       <c r="AH21" s="8"/>
       <c r="AI21" s="7"/>
       <c r="AJ21" s="7"/>
@@ -1953,12 +2000,8 @@
     <mergeCell ref="A1:AJ1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" xr:uid="{38DBEDAC-6A18-4D52-8516-7F6ACE1260D8}"/>
-    <hyperlink ref="C6" r:id="rId2" xr:uid="{F528F4DF-3477-4E50-98F5-E358FC6EF63E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2012,50 +2055,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="14"/>
-      <c r="AG1" s="14"/>
-      <c r="AH1" s="14"/>
-      <c r="AI1" s="14"/>
-      <c r="AJ1" s="14"/>
-      <c r="AK1" s="14"/>
-      <c r="AL1" s="14"/>
-      <c r="AM1" s="14"/>
-      <c r="AN1" s="14"/>
-      <c r="AO1" s="14"/>
-      <c r="AP1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="15"/>
+      <c r="AN1" s="15"/>
+      <c r="AO1" s="15"/>
+      <c r="AP1" s="15"/>
     </row>
     <row r="2" spans="1:42" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -3161,40 +3204,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="17"/>
     </row>
     <row r="2" spans="1:32" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -4141,131 +4184,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
     </row>
     <row r="2" spans="1:32" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
     </row>
     <row r="3" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="M3" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="N3" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="O3" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="P3" s="19" t="s">
+      <c r="P3" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19" t="s">
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="S3" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="T3" s="19" t="s">
+      <c r="T3" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="U3" s="19" t="s">
+      <c r="U3" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="V3" s="19" t="s">
+      <c r="V3" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="W3" s="19" t="s">
+      <c r="W3" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="X3" s="19" t="s">
+      <c r="X3" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="Y3" s="19" t="s">
+      <c r="Y3" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="Z3" s="19" t="s">
+      <c r="Z3" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="AA3" s="19" t="s">
+      <c r="AA3" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="AB3" s="19" t="s">
+      <c r="AB3" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="19"/>
-      <c r="AE3" s="19"/>
-      <c r="AF3" s="19"/>
+      <c r="AC3" s="13"/>
+      <c r="AD3" s="13"/>
+      <c r="AE3" s="13"/>
+      <c r="AF3" s="13"/>
     </row>
     <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">

</xml_diff>

<commit_message>
Login scenarios are added
</commit_message>
<xml_diff>
--- a/src/test/test_data/gigatron.xlsx
+++ b/src/test/test_data/gigatron.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\gigatron\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B456F263-B252-479F-A2F8-2A53B8469770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3501C3D9-CC2B-4D53-9451-A40B3B2A1E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="144">
   <si>
     <t>tc_id</t>
   </si>
@@ -36,9 +36,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>emptyEmailPasswordMessage2</t>
-  </si>
-  <si>
     <t>Test import data for "Ipon.hu" project</t>
   </si>
   <si>
@@ -448,6 +445,21 @@
   </si>
   <si>
     <t>https://gigatron.rs/korisnik</t>
+  </si>
+  <si>
+    <t>stjepanovics80</t>
+  </si>
+  <si>
+    <t>rgba(255, 0, 0, 1)</t>
+  </si>
+  <si>
+    <t>Kikinda</t>
+  </si>
+  <si>
+    <t>Došlo je do greške. Korisnik nije pronađen ili je neispravna lozinka.</t>
+  </si>
+  <si>
+    <t>stjep@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -647,6 +659,28 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -665,28 +699,8 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1009,250 +1023,248 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D05107-472F-4DD1-88F8-DE97CAF36E00}">
   <dimension ref="A1:AJ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="30" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="22" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="22" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="20" style="22" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" style="22" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" style="22" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="22" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="22" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" style="22" customWidth="1"/>
-    <col min="14" max="14" width="20" style="22" customWidth="1"/>
-    <col min="15" max="16" width="17.42578125" style="22" customWidth="1"/>
-    <col min="17" max="17" width="24" style="22" customWidth="1"/>
-    <col min="18" max="18" width="21.5703125" style="22" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" style="22" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" style="22" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" style="22" customWidth="1"/>
-    <col min="22" max="22" width="5.7109375" style="22" customWidth="1"/>
-    <col min="23" max="23" width="8" style="22" customWidth="1"/>
-    <col min="24" max="24" width="13" style="22" customWidth="1"/>
-    <col min="25" max="25" width="10.7109375" style="22" customWidth="1"/>
-    <col min="26" max="26" width="23.28515625" style="22" customWidth="1"/>
-    <col min="27" max="28" width="16.7109375" style="22" customWidth="1"/>
-    <col min="29" max="29" width="17.140625" style="22" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" style="22" customWidth="1"/>
-    <col min="31" max="31" width="16.140625" style="22" customWidth="1"/>
-    <col min="32" max="32" width="21.140625" style="22" customWidth="1"/>
-    <col min="33" max="33" width="30.85546875" style="22" customWidth="1"/>
-    <col min="34" max="34" width="17" style="22" customWidth="1"/>
-    <col min="35" max="35" width="15.7109375" style="22" customWidth="1"/>
-    <col min="36" max="36" width="14.42578125" style="22" customWidth="1"/>
-    <col min="37" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="1" width="8.140625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="14" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="20" style="14" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="14" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="14" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="14" customWidth="1"/>
+    <col min="14" max="14" width="20" style="14" customWidth="1"/>
+    <col min="15" max="16" width="17.42578125" style="14" customWidth="1"/>
+    <col min="17" max="17" width="24" style="14" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" style="14" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" style="14" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" style="14" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" style="14" customWidth="1"/>
+    <col min="22" max="22" width="5.7109375" style="14" customWidth="1"/>
+    <col min="23" max="23" width="8" style="14" customWidth="1"/>
+    <col min="24" max="24" width="13" style="14" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" style="14" customWidth="1"/>
+    <col min="26" max="26" width="23.28515625" style="14" customWidth="1"/>
+    <col min="27" max="28" width="16.7109375" style="14" customWidth="1"/>
+    <col min="29" max="29" width="17.140625" style="14" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="14" customWidth="1"/>
+    <col min="31" max="31" width="16.140625" style="14" customWidth="1"/>
+    <col min="32" max="32" width="21.140625" style="14" customWidth="1"/>
+    <col min="33" max="33" width="30.85546875" style="14" customWidth="1"/>
+    <col min="34" max="34" width="17" style="14" customWidth="1"/>
+    <col min="35" max="35" width="15.7109375" style="14" customWidth="1"/>
+    <col min="36" max="36" width="14.42578125" style="14" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="23"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="23"/>
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="23"/>
+      <c r="AJ1" s="23"/>
+    </row>
+    <row r="2" spans="1:36" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15"/>
+    </row>
+    <row r="3" spans="1:36" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="R3" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="S3" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="T3" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="U3" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="V3" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="W3" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="X3" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y3" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z3" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA3" s="16"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="16"/>
+      <c r="AH3" s="16"/>
+      <c r="AI3" s="16"/>
+      <c r="AJ3" s="16"/>
+    </row>
+    <row r="4" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="21"/>
-      <c r="AI1" s="21"/>
-      <c r="AJ1" s="21"/>
-    </row>
-    <row r="2" spans="1:36" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23"/>
-    </row>
-    <row r="3" spans="1:36" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="24" t="s">
+      <c r="B4" s="19" t="s">
         <v>138</v>
-      </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="N3" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="O3" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="P3" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q3" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="R3" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="S3" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="T3" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="U3" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="V3" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="W3" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="X3" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y3" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z3" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="AA3" s="24"/>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="24"/>
-      <c r="AD3" s="24"/>
-      <c r="AE3" s="24"/>
-      <c r="AF3" s="24"/>
-      <c r="AG3" s="24"/>
-      <c r="AH3" s="24"/>
-      <c r="AI3" s="24"/>
-      <c r="AJ3" s="24"/>
-    </row>
-    <row r="4" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>139</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>137</v>
+        <v>27</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>136</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>42</v>
+        <v>140</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N4" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="O4" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="P4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="Q4" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="R4" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="R4" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="S4" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="W4" s="7"/>
       <c r="X4" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Y4" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z4" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
@@ -1266,33 +1278,35 @@
       <c r="AJ4" s="7"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
-        <v>5</v>
+      <c r="A5" s="18" t="s">
+        <v>4</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>137</v>
+        <v>139</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>136</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="7"/>
+        <v>115</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>140</v>
+      </c>
       <c r="J5" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" s="28"/>
+        <v>38</v>
+      </c>
+      <c r="M5" s="19"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
@@ -1318,31 +1332,31 @@
       <c r="AJ5" s="7"/>
     </row>
     <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
-        <v>6</v>
+      <c r="A6" s="18" t="s">
+        <v>5</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>137</v>
+      <c r="D6" s="7"/>
+      <c r="E6" s="19" t="s">
+        <v>136</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="7"/>
+        <v>115</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>140</v>
+      </c>
       <c r="J6" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
-      <c r="M6" s="28"/>
+      <c r="M6" s="19"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -1368,31 +1382,33 @@
       <c r="AJ6" s="7"/>
     </row>
     <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
-        <v>7</v>
+      <c r="A7" s="18" t="s">
+        <v>6</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>34</v>
+        <v>27</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>142</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="7"/>
+        <v>115</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>140</v>
+      </c>
       <c r="J7" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="28"/>
+      <c r="M7" s="19"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
@@ -1418,38 +1434,38 @@
       <c r="AJ7" s="7"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
-        <v>8</v>
+      <c r="A8" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>137</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E8" s="19"/>
       <c r="F8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="7"/>
+        <v>115</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>140</v>
+      </c>
       <c r="J8" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="28"/>
+      <c r="M8" s="19"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="28"/>
-      <c r="T8" s="28"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
@@ -1467,30 +1483,34 @@
       <c r="AI8" s="7"/>
       <c r="AJ8" s="7"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
-        <v>9</v>
+    <row r="9" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
+        <v>8</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>34</v>
+      <c r="D9" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>142</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="7"/>
+        <v>115</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>140</v>
+      </c>
       <c r="J9" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="28"/>
+      <c r="M9" s="19"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
@@ -1516,8 +1536,8 @@
       <c r="AJ9" s="7"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
-        <v>10</v>
+      <c r="A10" s="18" t="s">
+        <v>9</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1556,8 +1576,8 @@
       <c r="AJ10" s="7"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
-        <v>11</v>
+      <c r="A11" s="18" t="s">
+        <v>10</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1570,34 +1590,34 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
-      <c r="M11" s="28"/>
+      <c r="M11" s="19"/>
       <c r="N11" s="7"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="28"/>
-      <c r="T11" s="28"/>
-      <c r="U11" s="28"/>
-      <c r="V11" s="28"/>
-      <c r="W11" s="28"/>
-      <c r="X11" s="28"/>
-      <c r="Y11" s="28"/>
-      <c r="Z11" s="28"/>
-      <c r="AA11" s="28"/>
-      <c r="AB11" s="28"/>
-      <c r="AC11" s="28"/>
-      <c r="AD11" s="28"/>
-      <c r="AE11" s="28"/>
-      <c r="AF11" s="28"/>
-      <c r="AG11" s="28"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="19"/>
+      <c r="AC11" s="19"/>
+      <c r="AD11" s="19"/>
+      <c r="AE11" s="19"/>
+      <c r="AF11" s="19"/>
+      <c r="AG11" s="19"/>
       <c r="AH11" s="7"/>
       <c r="AI11" s="7"/>
       <c r="AJ11" s="7"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
-        <v>12</v>
+      <c r="A12" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1609,39 +1629,39 @@
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="28"/>
-      <c r="T12" s="28"/>
-      <c r="U12" s="28"/>
-      <c r="V12" s="28"/>
-      <c r="W12" s="28"/>
-      <c r="X12" s="28"/>
-      <c r="Y12" s="28"/>
-      <c r="Z12" s="28"/>
-      <c r="AA12" s="28"/>
-      <c r="AB12" s="28"/>
-      <c r="AC12" s="28"/>
-      <c r="AD12" s="28"/>
-      <c r="AE12" s="28"/>
-      <c r="AF12" s="28"/>
-      <c r="AG12" s="28"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="19"/>
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="19"/>
+      <c r="AB12" s="19"/>
+      <c r="AC12" s="19"/>
+      <c r="AD12" s="19"/>
+      <c r="AE12" s="19"/>
+      <c r="AF12" s="19"/>
+      <c r="AG12" s="19"/>
       <c r="AH12" s="7"/>
       <c r="AI12" s="7"/>
       <c r="AJ12" s="7"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A13" s="26" t="s">
-        <v>13</v>
+      <c r="A13" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1651,35 +1671,35 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="28"/>
-      <c r="T13" s="28"/>
-      <c r="U13" s="28"/>
-      <c r="V13" s="28"/>
-      <c r="W13" s="28"/>
-      <c r="X13" s="28"/>
-      <c r="Y13" s="28"/>
-      <c r="Z13" s="28"/>
-      <c r="AA13" s="28"/>
-      <c r="AB13" s="28"/>
-      <c r="AC13" s="28"/>
-      <c r="AD13" s="28"/>
-      <c r="AE13" s="28"/>
-      <c r="AF13" s="28"/>
-      <c r="AG13" s="28"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
+      <c r="X13" s="19"/>
+      <c r="Y13" s="19"/>
+      <c r="Z13" s="19"/>
+      <c r="AA13" s="19"/>
+      <c r="AB13" s="19"/>
+      <c r="AC13" s="19"/>
+      <c r="AD13" s="19"/>
+      <c r="AE13" s="19"/>
+      <c r="AF13" s="19"/>
+      <c r="AG13" s="19"/>
       <c r="AH13" s="7"/>
       <c r="AI13" s="7"/>
       <c r="AJ13" s="7"/>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A14" s="26" t="s">
-        <v>14</v>
+      <c r="A14" s="18" t="s">
+        <v>13</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -1691,35 +1711,35 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="28"/>
-      <c r="R14" s="28"/>
-      <c r="S14" s="28"/>
-      <c r="T14" s="28"/>
-      <c r="U14" s="28"/>
-      <c r="V14" s="28"/>
-      <c r="W14" s="28"/>
-      <c r="X14" s="28"/>
-      <c r="Y14" s="28"/>
-      <c r="Z14" s="28"/>
-      <c r="AA14" s="28"/>
-      <c r="AB14" s="28"/>
-      <c r="AC14" s="28"/>
-      <c r="AD14" s="28"/>
-      <c r="AE14" s="28"/>
-      <c r="AF14" s="28"/>
-      <c r="AG14" s="28"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="19"/>
+      <c r="AC14" s="19"/>
+      <c r="AD14" s="19"/>
+      <c r="AE14" s="19"/>
+      <c r="AF14" s="19"/>
+      <c r="AG14" s="19"/>
       <c r="AH14" s="7"/>
       <c r="AI14" s="7"/>
       <c r="AJ14" s="7"/>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A15" s="26" t="s">
-        <v>15</v>
+      <c r="A15" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1731,35 +1751,35 @@
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="28"/>
-      <c r="S15" s="28"/>
-      <c r="T15" s="28"/>
-      <c r="U15" s="28"/>
-      <c r="V15" s="28"/>
-      <c r="W15" s="28"/>
-      <c r="X15" s="28"/>
-      <c r="Y15" s="28"/>
-      <c r="Z15" s="28"/>
-      <c r="AA15" s="28"/>
-      <c r="AB15" s="28"/>
-      <c r="AC15" s="28"/>
-      <c r="AD15" s="28"/>
-      <c r="AE15" s="28"/>
-      <c r="AF15" s="28"/>
-      <c r="AG15" s="28"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="19"/>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="19"/>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="19"/>
+      <c r="AB15" s="19"/>
+      <c r="AC15" s="19"/>
+      <c r="AD15" s="19"/>
+      <c r="AE15" s="19"/>
+      <c r="AF15" s="19"/>
+      <c r="AG15" s="19"/>
       <c r="AH15" s="7"/>
       <c r="AI15" s="7"/>
       <c r="AJ15" s="7"/>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
-        <v>16</v>
+      <c r="A16" s="18" t="s">
+        <v>15</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -1771,35 +1791,35 @@
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
-      <c r="R16" s="28"/>
-      <c r="S16" s="28"/>
-      <c r="T16" s="28"/>
-      <c r="U16" s="28"/>
-      <c r="V16" s="28"/>
-      <c r="W16" s="29"/>
-      <c r="X16" s="29"/>
-      <c r="Y16" s="29"/>
-      <c r="Z16" s="29"/>
-      <c r="AA16" s="29"/>
-      <c r="AB16" s="29"/>
-      <c r="AC16" s="29"/>
-      <c r="AD16" s="29"/>
-      <c r="AE16" s="29"/>
-      <c r="AF16" s="29"/>
-      <c r="AG16" s="29"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="20"/>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="20"/>
+      <c r="Z16" s="20"/>
+      <c r="AA16" s="20"/>
+      <c r="AB16" s="20"/>
+      <c r="AC16" s="20"/>
+      <c r="AD16" s="20"/>
+      <c r="AE16" s="20"/>
+      <c r="AF16" s="20"/>
+      <c r="AG16" s="20"/>
       <c r="AH16" s="8"/>
       <c r="AI16" s="7"/>
       <c r="AJ16" s="7"/>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A17" s="26" t="s">
-        <v>17</v>
+      <c r="A17" s="18" t="s">
+        <v>16</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1811,115 +1831,115 @@
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="28"/>
-      <c r="S17" s="28"/>
-      <c r="T17" s="28"/>
-      <c r="U17" s="28"/>
-      <c r="V17" s="28"/>
-      <c r="W17" s="28"/>
-      <c r="X17" s="28"/>
-      <c r="Y17" s="28"/>
-      <c r="Z17" s="28"/>
-      <c r="AA17" s="28"/>
-      <c r="AB17" s="28"/>
-      <c r="AC17" s="28"/>
-      <c r="AD17" s="28"/>
-      <c r="AE17" s="28"/>
-      <c r="AF17" s="28"/>
-      <c r="AG17" s="28"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
+      <c r="X17" s="19"/>
+      <c r="Y17" s="19"/>
+      <c r="Z17" s="19"/>
+      <c r="AA17" s="19"/>
+      <c r="AB17" s="19"/>
+      <c r="AC17" s="19"/>
+      <c r="AD17" s="19"/>
+      <c r="AE17" s="19"/>
+      <c r="AF17" s="19"/>
+      <c r="AG17" s="19"/>
       <c r="AH17" s="7"/>
       <c r="AI17" s="7"/>
       <c r="AJ17" s="7"/>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A18" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
+      <c r="A18" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="28"/>
-      <c r="S18" s="28"/>
-      <c r="T18" s="28"/>
-      <c r="U18" s="28"/>
-      <c r="V18" s="28"/>
-      <c r="W18" s="28"/>
-      <c r="X18" s="28"/>
-      <c r="Y18" s="28"/>
-      <c r="Z18" s="28"/>
-      <c r="AA18" s="28"/>
-      <c r="AB18" s="28"/>
-      <c r="AC18" s="28"/>
-      <c r="AD18" s="28"/>
-      <c r="AE18" s="28"/>
-      <c r="AF18" s="28"/>
-      <c r="AG18" s="28"/>
-      <c r="AH18" s="28"/>
-      <c r="AI18" s="28"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="19"/>
+      <c r="X18" s="19"/>
+      <c r="Y18" s="19"/>
+      <c r="Z18" s="19"/>
+      <c r="AA18" s="19"/>
+      <c r="AB18" s="19"/>
+      <c r="AC18" s="19"/>
+      <c r="AD18" s="19"/>
+      <c r="AE18" s="19"/>
+      <c r="AF18" s="19"/>
+      <c r="AG18" s="19"/>
+      <c r="AH18" s="19"/>
+      <c r="AI18" s="19"/>
       <c r="AJ18" s="7"/>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A19" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
+      <c r="A19" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="28"/>
-      <c r="S19" s="28"/>
-      <c r="T19" s="28"/>
-      <c r="U19" s="28"/>
-      <c r="V19" s="28"/>
-      <c r="W19" s="28"/>
-      <c r="X19" s="28"/>
-      <c r="Y19" s="28"/>
-      <c r="Z19" s="28"/>
-      <c r="AA19" s="28"/>
-      <c r="AB19" s="28"/>
-      <c r="AC19" s="28"/>
-      <c r="AD19" s="28"/>
-      <c r="AE19" s="28"/>
-      <c r="AF19" s="28"/>
-      <c r="AG19" s="28"/>
-      <c r="AH19" s="28"/>
-      <c r="AI19" s="28"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="19"/>
+      <c r="V19" s="19"/>
+      <c r="W19" s="19"/>
+      <c r="X19" s="19"/>
+      <c r="Y19" s="19"/>
+      <c r="Z19" s="19"/>
+      <c r="AA19" s="19"/>
+      <c r="AB19" s="19"/>
+      <c r="AC19" s="19"/>
+      <c r="AD19" s="19"/>
+      <c r="AE19" s="19"/>
+      <c r="AF19" s="19"/>
+      <c r="AG19" s="19"/>
+      <c r="AH19" s="19"/>
+      <c r="AI19" s="19"/>
       <c r="AJ19" s="7"/>
     </row>
     <row r="20" spans="1:36" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
-        <v>20</v>
+      <c r="A20" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1958,7 +1978,7 @@
       <c r="AJ20" s="7"/>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A21" s="26"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1969,28 +1989,28 @@
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="29"/>
-      <c r="S21" s="29"/>
-      <c r="T21" s="29"/>
-      <c r="U21" s="29"/>
-      <c r="V21" s="29"/>
-      <c r="W21" s="29"/>
-      <c r="X21" s="29"/>
-      <c r="Y21" s="29"/>
-      <c r="Z21" s="29"/>
-      <c r="AA21" s="29"/>
-      <c r="AB21" s="29"/>
-      <c r="AC21" s="29"/>
-      <c r="AD21" s="29"/>
-      <c r="AE21" s="29"/>
-      <c r="AF21" s="29"/>
-      <c r="AG21" s="29"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="20"/>
+      <c r="S21" s="20"/>
+      <c r="T21" s="20"/>
+      <c r="U21" s="20"/>
+      <c r="V21" s="20"/>
+      <c r="W21" s="20"/>
+      <c r="X21" s="20"/>
+      <c r="Y21" s="20"/>
+      <c r="Z21" s="20"/>
+      <c r="AA21" s="20"/>
+      <c r="AB21" s="20"/>
+      <c r="AC21" s="20"/>
+      <c r="AD21" s="20"/>
+      <c r="AE21" s="20"/>
+      <c r="AF21" s="20"/>
+      <c r="AG21" s="20"/>
       <c r="AH21" s="8"/>
       <c r="AI21" s="7"/>
       <c r="AJ21" s="7"/>
@@ -2055,50 +2075,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
+      <c r="A1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+      <c r="AO1" s="25"/>
+      <c r="AP1" s="25"/>
     </row>
     <row r="2" spans="1:42" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -2108,59 +2128,59 @@
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="S3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
@@ -2187,20 +2207,20 @@
     </row>
     <row r="4" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -2209,20 +2229,20 @@
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O4" s="7"/>
       <c r="P4" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
@@ -2251,50 +2271,50 @@
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D5" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
@@ -2323,22 +2343,22 @@
     </row>
     <row r="6" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -2347,17 +2367,17 @@
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
@@ -2385,46 +2405,46 @@
     </row>
     <row r="7" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D7" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
       <c r="S7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="T7" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="T7" s="7" t="s">
-        <v>56</v>
       </c>
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
@@ -2451,44 +2471,44 @@
     </row>
     <row r="8" spans="1:42" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U8" s="7"/>
       <c r="V8" s="5"/>
@@ -2515,46 +2535,46 @@
     </row>
     <row r="9" spans="1:42" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U9" s="7"/>
       <c r="V9" s="7"/>
@@ -2581,44 +2601,44 @@
     </row>
     <row r="10" spans="1:42" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D10" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L10" s="7"/>
       <c r="M10" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
       <c r="P10" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
       <c r="T10" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U10" s="7"/>
       <c r="V10" s="7"/>
@@ -2645,7 +2665,7 @@
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -2691,7 +2711,7 @@
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -2737,7 +2757,7 @@
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -2783,7 +2803,7 @@
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -2829,7 +2849,7 @@
     </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -2875,7 +2895,7 @@
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -2921,7 +2941,7 @@
     </row>
     <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -2967,7 +2987,7 @@
     </row>
     <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -3013,7 +3033,7 @@
     </row>
     <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -3059,7 +3079,7 @@
     </row>
     <row r="20" spans="1:42" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -3204,40 +3224,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17"/>
+      <c r="A1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="27"/>
     </row>
     <row r="2" spans="1:32" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -3247,64 +3267,64 @@
         <v>0</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K3" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="L3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="N3" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="N3" s="12" t="s">
-        <v>86</v>
-      </c>
       <c r="O3" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P3" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R3" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T3" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U3" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
@@ -3320,59 +3340,59 @@
     </row>
     <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D4" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I4" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="K4" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>94</v>
-      </c>
       <c r="N4" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P4" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="Q4" s="7"/>
       <c r="R4" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
@@ -3390,59 +3410,59 @@
     </row>
     <row r="5" spans="1:32" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D5" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I5" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J5" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="K5" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L5" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="O5" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="P5" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="P5" s="7" t="s">
-        <v>102</v>
-      </c>
       <c r="Q5" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
@@ -3460,33 +3480,33 @@
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D6" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -3495,10 +3515,10 @@
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T6" s="8"/>
       <c r="U6" s="8"/>
@@ -3516,61 +3536,61 @@
     </row>
     <row r="7" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D7" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J7" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="K7" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L7" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="M7" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="N7" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="O7" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="N7" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="O7" s="7" t="s">
+      <c r="P7" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="Q7" s="7"/>
       <c r="R7" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S7" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T7" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U7" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="V7" s="8"/>
       <c r="W7" s="8"/>
@@ -3586,58 +3606,58 @@
     </row>
     <row r="8" spans="1:32" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D8" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J8" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="K8" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L8" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="M8" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="N8" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="O8" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="N8" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="O8" s="7" t="s">
+      <c r="P8" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="Q8" s="7"/>
       <c r="R8" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S8" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T8" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
@@ -3654,23 +3674,23 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D9" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="5"/>
@@ -3700,7 +3720,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -3736,7 +3756,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -3772,7 +3792,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -3808,7 +3828,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -3844,7 +3864,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -3880,7 +3900,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -3916,7 +3936,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -3952,7 +3972,7 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -3988,7 +4008,7 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -4024,7 +4044,7 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -4060,7 +4080,7 @@
     </row>
     <row r="20" spans="1:32" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -4184,40 +4204,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
+      <c r="A1" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
     </row>
     <row r="2" spans="1:32" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -4227,83 +4247,83 @@
         <v>0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="L3" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="M3" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="N3" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="N3" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="O3" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q3" s="13"/>
       <c r="R3" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S3" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T3" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U3" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V3" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="W3" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="W3" s="13" t="s">
+      <c r="X3" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="X3" s="13" t="s">
-        <v>122</v>
-      </c>
       <c r="Y3" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z3" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="Z3" s="13" t="s">
-        <v>125</v>
-      </c>
       <c r="AA3" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB3" s="13" t="s">
         <v>118</v>
-      </c>
-      <c r="AB3" s="13" t="s">
-        <v>119</v>
       </c>
       <c r="AC3" s="13"/>
       <c r="AD3" s="13"/>
@@ -4312,74 +4332,74 @@
     </row>
     <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D4" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I4" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="K4" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>94</v>
-      </c>
       <c r="N4" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P4" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
       <c r="S4" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
       <c r="V4" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Y4" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Z4" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
@@ -4390,55 +4410,55 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D5" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I5" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J5" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="K5" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L5" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="O5" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="P5" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>102</v>
       </c>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
@@ -4455,33 +4475,33 @@
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D6" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -4491,7 +4511,7 @@
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T6" s="8"/>
       <c r="U6" s="8"/>
@@ -4509,68 +4529,68 @@
     </row>
     <row r="7" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D7" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J7" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="K7" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L7" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="M7" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="N7" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="O7" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="N7" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="O7" s="7" t="s">
+      <c r="P7" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
       <c r="S7" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T7" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U7" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="V7" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W7" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="X7" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
@@ -4583,56 +4603,56 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D8" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J8" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="K8" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L8" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="M8" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="N8" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="O8" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="N8" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="O8" s="7" t="s">
+      <c r="P8" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T8" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U8" s="7"/>
       <c r="W8" s="7"/>
@@ -4648,23 +4668,23 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D9" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="5"/>
@@ -4694,7 +4714,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -4730,7 +4750,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -4766,7 +4786,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -4802,7 +4822,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -4838,7 +4858,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -4874,7 +4894,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -4910,7 +4930,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -4946,7 +4966,7 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -4982,7 +5002,7 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -5018,7 +5038,7 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -5054,7 +5074,7 @@
     </row>
     <row r="20" spans="1:32" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>

</xml_diff>

<commit_message>
adresa dostave page is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/gigatron.xlsx
+++ b/src/test/test_data/gigatron.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\gigatron\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EEDB75-1F15-4CE0-8CC8-42D15F2E6E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B212D844-4428-4CC5-9B09-37D2E4A22AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <sheet name="checkout" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="143">
   <si>
     <t>tc_id</t>
   </si>
@@ -431,6 +430,33 @@
   </si>
   <si>
     <t>popod</t>
+  </si>
+  <si>
+    <t>https://gigatron.rs/korisnik/adresa-dostave</t>
+  </si>
+  <si>
+    <t>Sasa Stjepanovic</t>
+  </si>
+  <si>
+    <t>Hajduk Veljkova 44</t>
+  </si>
+  <si>
+    <t>11000 Beograd</t>
+  </si>
+  <si>
+    <t>0641234567</t>
+  </si>
+  <si>
+    <t>successMessage</t>
+  </si>
+  <si>
+    <t>`Obriši unos</t>
+  </si>
+  <si>
+    <t>email2</t>
+  </si>
+  <si>
+    <t>Nikola</t>
   </si>
 </sst>
 </file>
@@ -647,6 +673,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -664,9 +693,6 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1033,44 +1059,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
     </row>
     <row r="2" spans="1:36" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
@@ -1996,14 +2022,14 @@
   <dimension ref="A1:AJ21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="20" customWidth="1"/>
     <col min="2" max="2" width="28" style="13" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="16" style="13" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" style="13" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" style="13" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" style="13" customWidth="1"/>
@@ -2039,44 +2065,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
     </row>
     <row r="2" spans="1:36" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
@@ -2088,7 +2114,9 @@
       <c r="B3" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>139</v>
+      </c>
       <c r="D3" s="15" t="s">
         <v>26</v>
       </c>
@@ -2111,7 +2139,7 @@
         <v>105</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>33</v>
+        <v>141</v>
       </c>
       <c r="L3" s="15" t="s">
         <v>34</v>
@@ -2169,7 +2197,7 @@
       <c r="A4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="23" t="s">
         <v>122</v>
       </c>
       <c r="C4" s="6"/>
@@ -2247,7 +2275,7 @@
       <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="23" t="s">
         <v>122</v>
       </c>
       <c r="C5" s="6"/>
@@ -2301,7 +2329,7 @@
       <c r="A6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="23" t="s">
         <v>122</v>
       </c>
       <c r="C6" s="6"/>
@@ -2349,7 +2377,7 @@
       <c r="A7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="23" t="s">
         <v>122</v>
       </c>
       <c r="C7" s="6"/>
@@ -2397,7 +2425,7 @@
       <c r="A8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="23" t="s">
         <v>122</v>
       </c>
       <c r="C8" s="6"/>
@@ -2445,7 +2473,7 @@
       <c r="A9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="23" t="s">
         <v>122</v>
       </c>
       <c r="C9" s="6"/>
@@ -2493,7 +2521,7 @@
       <c r="A10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="23" t="s">
         <v>122</v>
       </c>
       <c r="C10" s="6"/>
@@ -2543,7 +2571,7 @@
       <c r="A11" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="23" t="s">
         <v>122</v>
       </c>
       <c r="C11" s="6"/>
@@ -2593,7 +2621,7 @@
       <c r="A12" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="23" t="s">
         <v>122</v>
       </c>
       <c r="C12" s="6"/>
@@ -2639,15 +2667,15 @@
       <c r="AI12" s="6"/>
       <c r="AJ12" s="6"/>
     </row>
-    <row r="13" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>122</v>
+      <c r="B13" s="23" t="s">
+        <v>134</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>27</v>
@@ -2656,11 +2684,21 @@
         <v>113</v>
       </c>
       <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+      <c r="G13" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="L13" s="18"/>
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
@@ -2691,8 +2729,8 @@
       <c r="A14" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="29" t="s">
-        <v>122</v>
+      <c r="B14" s="23" t="s">
+        <v>134</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6" t="s">
@@ -2701,7 +2739,9 @@
       <c r="E14" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -2737,8 +2777,8 @@
       <c r="A15" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="29" t="s">
-        <v>122</v>
+      <c r="B15" s="23" t="s">
+        <v>134</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6" t="s">
@@ -2747,7 +2787,9 @@
       <c r="E15" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -2783,8 +2825,8 @@
       <c r="A16" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="29" t="s">
-        <v>122</v>
+      <c r="B16" s="23" t="s">
+        <v>134</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6" t="s">
@@ -2793,8 +2835,12 @@
       <c r="E16" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>142</v>
+      </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
@@ -2829,8 +2875,8 @@
       <c r="A17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="29" t="s">
-        <v>122</v>
+      <c r="B17" s="23" t="s">
+        <v>134</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6" t="s">
@@ -2875,8 +2921,8 @@
       <c r="A18" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="29" t="s">
-        <v>122</v>
+      <c r="B18" s="23" t="s">
+        <v>134</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="6" t="s">
@@ -2921,8 +2967,8 @@
       <c r="A19" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="29" t="s">
-        <v>122</v>
+      <c r="B19" s="23" t="s">
+        <v>134</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="6" t="s">
@@ -3095,40 +3141,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="27"/>
     </row>
     <row r="2" spans="1:32" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
@@ -4075,40 +4121,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
     </row>
     <row r="2" spans="1:32" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>

</xml_diff>

<commit_message>
logic of filtering products is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/gigatron.xlsx
+++ b/src/test/test_data/gigatron.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\gigatron\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B212D844-4428-4CC5-9B09-37D2E4A22AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C4FE60-0C90-4C12-ABE3-89F30DEE2CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="4" r:id="rId1"/>
     <sheet name="korisnik" sheetId="5" r:id="rId2"/>
-    <sheet name="notebook" sheetId="6" r:id="rId3"/>
+    <sheet name="laptop" sheetId="6" r:id="rId3"/>
     <sheet name="checkout" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="148">
   <si>
     <t>tc_id</t>
   </si>
@@ -267,12 +267,6 @@
     <t>19</t>
   </si>
   <si>
-    <t>noFilteredAction</t>
-  </si>
-  <si>
-    <t>Sadly, there is no result we can show you!</t>
-  </si>
-  <si>
     <t>LENOVO</t>
   </si>
   <si>
@@ -291,9 +285,6 @@
     <t>emptyBasket</t>
   </si>
   <si>
-    <t>YOUR CART IS EMPTY!</t>
-  </si>
-  <si>
     <t>quantity</t>
   </si>
   <si>
@@ -457,6 +448,30 @@
   </si>
   <si>
     <t>Nikola</t>
+  </si>
+  <si>
+    <t>Proizvođač</t>
+  </si>
+  <si>
+    <t>Gaming</t>
+  </si>
+  <si>
+    <t>Acer</t>
+  </si>
+  <si>
+    <t>Da</t>
+  </si>
+  <si>
+    <t>filter1</t>
+  </si>
+  <si>
+    <t>filter2</t>
+  </si>
+  <si>
+    <t>value1</t>
+  </si>
+  <si>
+    <t>value2</t>
   </si>
 </sst>
 </file>
@@ -544,7 +559,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,12 +575,6 @@
           <color theme="5" tint="0.40000610370189521"/>
         </stop>
       </gradientFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor auto="1"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -623,7 +632,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -648,9 +657,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -686,12 +692,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1021,193 +1021,193 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="18" style="13" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="13" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="20" style="13" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" style="13" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="13" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="13" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" style="13" customWidth="1"/>
-    <col min="14" max="14" width="20" style="13" customWidth="1"/>
-    <col min="15" max="16" width="17.42578125" style="13" customWidth="1"/>
-    <col min="17" max="17" width="24" style="13" customWidth="1"/>
-    <col min="18" max="18" width="21.5703125" style="13" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" style="13" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" style="13" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" style="13" customWidth="1"/>
-    <col min="22" max="22" width="5.7109375" style="13" customWidth="1"/>
-    <col min="23" max="23" width="8" style="13" customWidth="1"/>
-    <col min="24" max="24" width="13" style="13" customWidth="1"/>
-    <col min="25" max="25" width="10.7109375" style="13" customWidth="1"/>
-    <col min="26" max="26" width="23.28515625" style="13" customWidth="1"/>
-    <col min="27" max="28" width="16.7109375" style="13" customWidth="1"/>
-    <col min="29" max="29" width="17.140625" style="13" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" style="13" customWidth="1"/>
-    <col min="31" max="31" width="16.140625" style="13" customWidth="1"/>
-    <col min="32" max="32" width="21.140625" style="13" customWidth="1"/>
-    <col min="33" max="33" width="30.85546875" style="13" customWidth="1"/>
-    <col min="34" max="34" width="17" style="13" customWidth="1"/>
-    <col min="35" max="35" width="15.7109375" style="13" customWidth="1"/>
-    <col min="36" max="36" width="14.42578125" style="13" customWidth="1"/>
-    <col min="37" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="8.140625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="18" style="12" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="20" style="12" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="12" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="12" customWidth="1"/>
+    <col min="14" max="14" width="20" style="12" customWidth="1"/>
+    <col min="15" max="16" width="17.42578125" style="12" customWidth="1"/>
+    <col min="17" max="17" width="24" style="12" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" style="12" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" style="12" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" style="12" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" style="12" customWidth="1"/>
+    <col min="22" max="22" width="5.7109375" style="12" customWidth="1"/>
+    <col min="23" max="23" width="8" style="12" customWidth="1"/>
+    <col min="24" max="24" width="13" style="12" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" style="12" customWidth="1"/>
+    <col min="26" max="26" width="23.28515625" style="12" customWidth="1"/>
+    <col min="27" max="28" width="16.7109375" style="12" customWidth="1"/>
+    <col min="29" max="29" width="17.140625" style="12" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="12" customWidth="1"/>
+    <col min="31" max="31" width="16.140625" style="12" customWidth="1"/>
+    <col min="32" max="32" width="21.140625" style="12" customWidth="1"/>
+    <col min="33" max="33" width="30.85546875" style="12" customWidth="1"/>
+    <col min="34" max="34" width="17" style="12" customWidth="1"/>
+    <col min="35" max="35" width="15.7109375" style="12" customWidth="1"/>
+    <col min="36" max="36" width="14.42578125" style="12" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="A1" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
     </row>
     <row r="2" spans="1:36" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-    </row>
-    <row r="3" spans="1:36" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A2" s="13"/>
+    </row>
+    <row r="3" spans="1:36" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15" t="s">
+      <c r="B3" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="I3" s="15" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="T3" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="U3" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="V3" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="W3" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="X3" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="J3" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="N3" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="O3" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q3" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="R3" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="S3" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="T3" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="U3" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="V3" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="W3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="X3" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y3" s="15" t="s">
+      <c r="Y3" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z3" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="Z3" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="15"/>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="15"/>
-      <c r="AG3" s="15"/>
-      <c r="AH3" s="15"/>
-      <c r="AI3" s="15"/>
-      <c r="AJ3" s="15"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="14"/>
+      <c r="AF3" s="14"/>
+      <c r="AG3" s="14"/>
+      <c r="AH3" s="14"/>
+      <c r="AI3" s="14"/>
+      <c r="AJ3" s="14"/>
     </row>
     <row r="4" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>115</v>
+      <c r="B4" s="21" t="s">
+        <v>112</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>113</v>
+      <c r="E4" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>25</v>
@@ -1243,20 +1243,20 @@
         <v>54</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="W4" s="6"/>
       <c r="X4" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
@@ -1270,24 +1270,24 @@
       <c r="AJ4" s="6"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E5" s="18" t="s">
         <v>113</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>25</v>
@@ -1298,7 +1298,7 @@
       <c r="L5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="18"/>
+      <c r="M5" s="17"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
@@ -1324,31 +1324,31 @@
       <c r="AJ5" s="6"/>
     </row>
     <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="18" t="s">
-        <v>113</v>
+      <c r="E6" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>31</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>25</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="18"/>
+      <c r="M6" s="17"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
@@ -1374,7 +1374,7 @@
       <c r="AJ6" s="6"/>
     </row>
     <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="6"/>
@@ -1382,25 +1382,25 @@
       <c r="D7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>119</v>
+      <c r="E7" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>116</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J7" s="10" t="s">
         <v>25</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-      <c r="M7" s="18"/>
+      <c r="M7" s="17"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
@@ -1426,7 +1426,7 @@
       <c r="AJ7" s="6"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="6"/>
@@ -1434,30 +1434,30 @@
       <c r="D8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="18"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="6" t="s">
         <v>31</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>25</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="18"/>
+      <c r="M8" s="17"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
@@ -1476,33 +1476,33 @@
       <c r="AJ8" s="6"/>
     </row>
     <row r="9" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>119</v>
+      <c r="D9" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>116</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>25</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
-      <c r="M9" s="18"/>
+      <c r="M9" s="17"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
@@ -1528,7 +1528,7 @@
       <c r="AJ9" s="6"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="6"/>
@@ -1568,7 +1568,7 @@
       <c r="AJ10" s="6"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="6"/>
@@ -1582,33 +1582,33 @@
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
-      <c r="M11" s="18"/>
+      <c r="M11" s="17"/>
       <c r="N11" s="6"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="18"/>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="18"/>
-      <c r="AC11" s="18"/>
-      <c r="AD11" s="18"/>
-      <c r="AE11" s="18"/>
-      <c r="AF11" s="18"/>
-      <c r="AG11" s="18"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
+      <c r="AA11" s="17"/>
+      <c r="AB11" s="17"/>
+      <c r="AC11" s="17"/>
+      <c r="AD11" s="17"/>
+      <c r="AE11" s="17"/>
+      <c r="AF11" s="17"/>
+      <c r="AG11" s="17"/>
       <c r="AH11" s="6"/>
       <c r="AI11" s="6"/>
       <c r="AJ11" s="6"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="6"/>
@@ -1621,39 +1621,39 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="18"/>
-      <c r="AA12" s="18"/>
-      <c r="AB12" s="18"/>
-      <c r="AC12" s="18"/>
-      <c r="AD12" s="18"/>
-      <c r="AE12" s="18"/>
-      <c r="AF12" s="18"/>
-      <c r="AG12" s="18"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="17"/>
+      <c r="AA12" s="17"/>
+      <c r="AB12" s="17"/>
+      <c r="AC12" s="17"/>
+      <c r="AD12" s="17"/>
+      <c r="AE12" s="17"/>
+      <c r="AF12" s="17"/>
+      <c r="AG12" s="17"/>
       <c r="AH12" s="6"/>
       <c r="AI12" s="6"/>
       <c r="AJ12" s="6"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1663,34 +1663,34 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
-      <c r="AA13" s="18"/>
-      <c r="AB13" s="18"/>
-      <c r="AC13" s="18"/>
-      <c r="AD13" s="18"/>
-      <c r="AE13" s="18"/>
-      <c r="AF13" s="18"/>
-      <c r="AG13" s="18"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="17"/>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17"/>
+      <c r="AA13" s="17"/>
+      <c r="AB13" s="17"/>
+      <c r="AC13" s="17"/>
+      <c r="AD13" s="17"/>
+      <c r="AE13" s="17"/>
+      <c r="AF13" s="17"/>
+      <c r="AG13" s="17"/>
       <c r="AH13" s="6"/>
       <c r="AI13" s="6"/>
       <c r="AJ13" s="6"/>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="6"/>
@@ -1703,34 +1703,34 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="18"/>
-      <c r="AA14" s="18"/>
-      <c r="AB14" s="18"/>
-      <c r="AC14" s="18"/>
-      <c r="AD14" s="18"/>
-      <c r="AE14" s="18"/>
-      <c r="AF14" s="18"/>
-      <c r="AG14" s="18"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="17"/>
+      <c r="AA14" s="17"/>
+      <c r="AB14" s="17"/>
+      <c r="AC14" s="17"/>
+      <c r="AD14" s="17"/>
+      <c r="AE14" s="17"/>
+      <c r="AF14" s="17"/>
+      <c r="AG14" s="17"/>
       <c r="AH14" s="6"/>
       <c r="AI14" s="6"/>
       <c r="AJ14" s="6"/>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="6"/>
@@ -1743,34 +1743,34 @@
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="18"/>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="18"/>
-      <c r="Z15" s="18"/>
-      <c r="AA15" s="18"/>
-      <c r="AB15" s="18"/>
-      <c r="AC15" s="18"/>
-      <c r="AD15" s="18"/>
-      <c r="AE15" s="18"/>
-      <c r="AF15" s="18"/>
-      <c r="AG15" s="18"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="17"/>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="17"/>
+      <c r="AE15" s="17"/>
+      <c r="AF15" s="17"/>
+      <c r="AG15" s="17"/>
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
       <c r="AJ15" s="6"/>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="6"/>
@@ -1783,34 +1783,34 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="19"/>
-      <c r="X16" s="19"/>
-      <c r="Y16" s="19"/>
-      <c r="Z16" s="19"/>
-      <c r="AA16" s="19"/>
-      <c r="AB16" s="19"/>
-      <c r="AC16" s="19"/>
-      <c r="AD16" s="19"/>
-      <c r="AE16" s="19"/>
-      <c r="AF16" s="19"/>
-      <c r="AG16" s="19"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="18"/>
+      <c r="Y16" s="18"/>
+      <c r="Z16" s="18"/>
+      <c r="AA16" s="18"/>
+      <c r="AB16" s="18"/>
+      <c r="AC16" s="18"/>
+      <c r="AD16" s="18"/>
+      <c r="AE16" s="18"/>
+      <c r="AF16" s="18"/>
+      <c r="AG16" s="18"/>
       <c r="AH16" s="7"/>
       <c r="AI16" s="6"/>
       <c r="AJ16" s="6"/>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="6"/>
@@ -1823,114 +1823,114 @@
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
-      <c r="W17" s="18"/>
-      <c r="X17" s="18"/>
-      <c r="Y17" s="18"/>
-      <c r="Z17" s="18"/>
-      <c r="AA17" s="18"/>
-      <c r="AB17" s="18"/>
-      <c r="AC17" s="18"/>
-      <c r="AD17" s="18"/>
-      <c r="AE17" s="18"/>
-      <c r="AF17" s="18"/>
-      <c r="AG17" s="18"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="17"/>
+      <c r="Y17" s="17"/>
+      <c r="Z17" s="17"/>
+      <c r="AA17" s="17"/>
+      <c r="AB17" s="17"/>
+      <c r="AC17" s="17"/>
+      <c r="AD17" s="17"/>
+      <c r="AE17" s="17"/>
+      <c r="AF17" s="17"/>
+      <c r="AG17" s="17"/>
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
       <c r="AJ17" s="6"/>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
-      <c r="X18" s="18"/>
-      <c r="Y18" s="18"/>
-      <c r="Z18" s="18"/>
-      <c r="AA18" s="18"/>
-      <c r="AB18" s="18"/>
-      <c r="AC18" s="18"/>
-      <c r="AD18" s="18"/>
-      <c r="AE18" s="18"/>
-      <c r="AF18" s="18"/>
-      <c r="AG18" s="18"/>
-      <c r="AH18" s="18"/>
-      <c r="AI18" s="18"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="17"/>
+      <c r="AA18" s="17"/>
+      <c r="AB18" s="17"/>
+      <c r="AC18" s="17"/>
+      <c r="AD18" s="17"/>
+      <c r="AE18" s="17"/>
+      <c r="AF18" s="17"/>
+      <c r="AG18" s="17"/>
+      <c r="AH18" s="17"/>
+      <c r="AI18" s="17"/>
       <c r="AJ18" s="6"/>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="18"/>
-      <c r="V19" s="18"/>
-      <c r="W19" s="18"/>
-      <c r="X19" s="18"/>
-      <c r="Y19" s="18"/>
-      <c r="Z19" s="18"/>
-      <c r="AA19" s="18"/>
-      <c r="AB19" s="18"/>
-      <c r="AC19" s="18"/>
-      <c r="AD19" s="18"/>
-      <c r="AE19" s="18"/>
-      <c r="AF19" s="18"/>
-      <c r="AG19" s="18"/>
-      <c r="AH19" s="18"/>
-      <c r="AI19" s="18"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="17"/>
+      <c r="AA19" s="17"/>
+      <c r="AB19" s="17"/>
+      <c r="AC19" s="17"/>
+      <c r="AD19" s="17"/>
+      <c r="AE19" s="17"/>
+      <c r="AF19" s="17"/>
+      <c r="AG19" s="17"/>
+      <c r="AH19" s="17"/>
+      <c r="AI19" s="17"/>
       <c r="AJ19" s="6"/>
     </row>
     <row r="20" spans="1:36" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="6"/>
@@ -1970,7 +1970,7 @@
       <c r="AJ20" s="6"/>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1981,28 +1981,28 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
-      <c r="S21" s="19"/>
-      <c r="T21" s="19"/>
-      <c r="U21" s="19"/>
-      <c r="V21" s="19"/>
-      <c r="W21" s="19"/>
-      <c r="X21" s="19"/>
-      <c r="Y21" s="19"/>
-      <c r="Z21" s="19"/>
-      <c r="AA21" s="19"/>
-      <c r="AB21" s="19"/>
-      <c r="AC21" s="19"/>
-      <c r="AD21" s="19"/>
-      <c r="AE21" s="19"/>
-      <c r="AF21" s="19"/>
-      <c r="AG21" s="19"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="18"/>
+      <c r="V21" s="18"/>
+      <c r="W21" s="18"/>
+      <c r="X21" s="18"/>
+      <c r="Y21" s="18"/>
+      <c r="Z21" s="18"/>
+      <c r="AA21" s="18"/>
+      <c r="AB21" s="18"/>
+      <c r="AC21" s="18"/>
+      <c r="AD21" s="18"/>
+      <c r="AE21" s="18"/>
+      <c r="AF21" s="18"/>
+      <c r="AG21" s="18"/>
       <c r="AH21" s="7"/>
       <c r="AI21" s="6"/>
       <c r="AJ21" s="6"/>
@@ -2021,194 +2021,194 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B244FFE7-0967-47E4-BD24-686C74F1C03E}">
   <dimension ref="A1:AJ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="28" style="13" customWidth="1"/>
-    <col min="3" max="3" width="16" style="13" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="13" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="13" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="13" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" style="13" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="13" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="13" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" style="13" customWidth="1"/>
-    <col min="14" max="14" width="20" style="13" customWidth="1"/>
-    <col min="15" max="16" width="17.42578125" style="13" customWidth="1"/>
-    <col min="17" max="17" width="24" style="13" customWidth="1"/>
-    <col min="18" max="18" width="21.5703125" style="13" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" style="13" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" style="13" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" style="13" customWidth="1"/>
-    <col min="22" max="22" width="5.7109375" style="13" customWidth="1"/>
-    <col min="23" max="23" width="8" style="13" customWidth="1"/>
-    <col min="24" max="24" width="13" style="13" customWidth="1"/>
-    <col min="25" max="25" width="10.7109375" style="13" customWidth="1"/>
-    <col min="26" max="26" width="23.28515625" style="13" customWidth="1"/>
-    <col min="27" max="28" width="16.7109375" style="13" customWidth="1"/>
-    <col min="29" max="29" width="17.140625" style="13" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" style="13" customWidth="1"/>
-    <col min="31" max="31" width="16.140625" style="13" customWidth="1"/>
-    <col min="32" max="32" width="21.140625" style="13" customWidth="1"/>
-    <col min="33" max="33" width="30.85546875" style="13" customWidth="1"/>
-    <col min="34" max="34" width="17" style="13" customWidth="1"/>
-    <col min="35" max="35" width="15.7109375" style="13" customWidth="1"/>
-    <col min="36" max="36" width="14.42578125" style="13" customWidth="1"/>
-    <col min="37" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="8.140625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="28" style="12" customWidth="1"/>
+    <col min="3" max="3" width="16" style="12" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="12" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="12" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="12" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="12" customWidth="1"/>
+    <col min="14" max="14" width="20" style="12" customWidth="1"/>
+    <col min="15" max="16" width="17.42578125" style="12" customWidth="1"/>
+    <col min="17" max="17" width="24" style="12" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" style="12" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" style="12" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" style="12" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" style="12" customWidth="1"/>
+    <col min="22" max="22" width="5.7109375" style="12" customWidth="1"/>
+    <col min="23" max="23" width="8" style="12" customWidth="1"/>
+    <col min="24" max="24" width="13" style="12" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" style="12" customWidth="1"/>
+    <col min="26" max="26" width="23.28515625" style="12" customWidth="1"/>
+    <col min="27" max="28" width="16.7109375" style="12" customWidth="1"/>
+    <col min="29" max="29" width="17.140625" style="12" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="12" customWidth="1"/>
+    <col min="31" max="31" width="16.140625" style="12" customWidth="1"/>
+    <col min="32" max="32" width="21.140625" style="12" customWidth="1"/>
+    <col min="33" max="33" width="30.85546875" style="12" customWidth="1"/>
+    <col min="34" max="34" width="17" style="12" customWidth="1"/>
+    <col min="35" max="35" width="15.7109375" style="12" customWidth="1"/>
+    <col min="36" max="36" width="14.42578125" style="12" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+    </row>
+    <row r="2" spans="1:36" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13"/>
+    </row>
+    <row r="3" spans="1:36" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
-    </row>
-    <row r="2" spans="1:36" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-    </row>
-    <row r="3" spans="1:36" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="T3" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="W3" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="X3" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="N3" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="O3" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q3" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="R3" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="S3" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="T3" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="W3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="X3" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y3" s="15"/>
-      <c r="Z3" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="15"/>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="15"/>
-      <c r="AG3" s="15"/>
-      <c r="AH3" s="15"/>
-      <c r="AI3" s="15"/>
-      <c r="AJ3" s="15"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="14"/>
+      <c r="AF3" s="14"/>
+      <c r="AG3" s="14"/>
+      <c r="AH3" s="14"/>
+      <c r="AI3" s="14"/>
+      <c r="AJ3" s="14"/>
     </row>
     <row r="4" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>122</v>
+      <c r="B4" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>113</v>
+      <c r="E4" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -2245,20 +2245,20 @@
         <v>54</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="W4" s="6"/>
       <c r="X4" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
@@ -2272,24 +2272,24 @@
       <c r="AJ4" s="6"/>
     </row>
     <row r="5" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>122</v>
+      <c r="B5" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>113</v>
+      <c r="E5" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -2300,7 +2300,7 @@
       <c r="L5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="18"/>
+      <c r="M5" s="17"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
@@ -2326,18 +2326,18 @@
       <c r="AJ5" s="6"/>
     </row>
     <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="23" t="s">
-        <v>122</v>
+      <c r="B6" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>113</v>
+      <c r="E6" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>31</v>
@@ -2348,7 +2348,7 @@
       <c r="J6" s="10"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="18"/>
+      <c r="M6" s="17"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
@@ -2374,21 +2374,21 @@
       <c r="AJ6" s="6"/>
     </row>
     <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>122</v>
+      <c r="B7" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>119</v>
+      <c r="E7" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>116</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -2396,7 +2396,7 @@
       <c r="J7" s="10"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-      <c r="M7" s="18"/>
+      <c r="M7" s="17"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
@@ -2422,18 +2422,18 @@
       <c r="AJ7" s="6"/>
     </row>
     <row r="8" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>122</v>
+      <c r="B8" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>113</v>
+      <c r="E8" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>31</v>
@@ -2444,14 +2444,14 @@
       <c r="J8" s="10"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="18"/>
+      <c r="M8" s="17"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
@@ -2470,21 +2470,21 @@
       <c r="AJ8" s="6"/>
     </row>
     <row r="9" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>122</v>
+      <c r="B9" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>119</v>
+      <c r="E9" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>116</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -2492,7 +2492,7 @@
       <c r="J9" s="10"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
-      <c r="M9" s="18"/>
+      <c r="M9" s="17"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
@@ -2518,26 +2518,26 @@
       <c r="AJ9" s="6"/>
     </row>
     <row r="10" spans="1:36" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>122</v>
+      <c r="B10" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="18" t="s">
-        <v>113</v>
+      <c r="E10" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -2568,322 +2568,322 @@
       <c r="AJ10" s="6"/>
     </row>
     <row r="11" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>122</v>
+      <c r="B11" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>113</v>
+      <c r="E11" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
-      <c r="M11" s="18"/>
+      <c r="M11" s="17"/>
       <c r="N11" s="6"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="18"/>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="18"/>
-      <c r="AC11" s="18"/>
-      <c r="AD11" s="18"/>
-      <c r="AE11" s="18"/>
-      <c r="AF11" s="18"/>
-      <c r="AG11" s="18"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
+      <c r="AA11" s="17"/>
+      <c r="AB11" s="17"/>
+      <c r="AC11" s="17"/>
+      <c r="AD11" s="17"/>
+      <c r="AE11" s="17"/>
+      <c r="AF11" s="17"/>
+      <c r="AG11" s="17"/>
       <c r="AH11" s="6"/>
       <c r="AI11" s="6"/>
       <c r="AJ11" s="6"/>
     </row>
     <row r="12" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="23" t="s">
-        <v>122</v>
+      <c r="B12" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>113</v>
+      <c r="E12" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K12" s="6"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="18"/>
-      <c r="AA12" s="18"/>
-      <c r="AB12" s="18"/>
-      <c r="AC12" s="18"/>
-      <c r="AD12" s="18"/>
-      <c r="AE12" s="18"/>
-      <c r="AF12" s="18"/>
-      <c r="AG12" s="18"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="17"/>
+      <c r="AA12" s="17"/>
+      <c r="AB12" s="17"/>
+      <c r="AC12" s="17"/>
+      <c r="AD12" s="17"/>
+      <c r="AE12" s="17"/>
+      <c r="AF12" s="17"/>
+      <c r="AG12" s="17"/>
       <c r="AH12" s="6"/>
       <c r="AI12" s="6"/>
       <c r="AJ12" s="6"/>
     </row>
     <row r="13" spans="1:36" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>134</v>
+      <c r="B13" s="22" t="s">
+        <v>131</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="18" t="s">
-        <v>113</v>
+      <c r="E13" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>138</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
-      <c r="AA13" s="18"/>
-      <c r="AB13" s="18"/>
-      <c r="AC13" s="18"/>
-      <c r="AD13" s="18"/>
-      <c r="AE13" s="18"/>
-      <c r="AF13" s="18"/>
-      <c r="AG13" s="18"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="17"/>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17"/>
+      <c r="AA13" s="17"/>
+      <c r="AB13" s="17"/>
+      <c r="AC13" s="17"/>
+      <c r="AD13" s="17"/>
+      <c r="AE13" s="17"/>
+      <c r="AF13" s="17"/>
+      <c r="AG13" s="17"/>
       <c r="AH13" s="6"/>
       <c r="AI13" s="6"/>
       <c r="AJ13" s="6"/>
     </row>
     <row r="14" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="23" t="s">
-        <v>134</v>
+      <c r="B14" s="22" t="s">
+        <v>131</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="18" t="s">
-        <v>113</v>
+      <c r="E14" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="18"/>
-      <c r="AA14" s="18"/>
-      <c r="AB14" s="18"/>
-      <c r="AC14" s="18"/>
-      <c r="AD14" s="18"/>
-      <c r="AE14" s="18"/>
-      <c r="AF14" s="18"/>
-      <c r="AG14" s="18"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="17"/>
+      <c r="AA14" s="17"/>
+      <c r="AB14" s="17"/>
+      <c r="AC14" s="17"/>
+      <c r="AD14" s="17"/>
+      <c r="AE14" s="17"/>
+      <c r="AF14" s="17"/>
+      <c r="AG14" s="17"/>
       <c r="AH14" s="6"/>
       <c r="AI14" s="6"/>
       <c r="AJ14" s="6"/>
     </row>
     <row r="15" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="23" t="s">
-        <v>134</v>
+      <c r="B15" s="22" t="s">
+        <v>131</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="18" t="s">
-        <v>113</v>
+      <c r="E15" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="18"/>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="18"/>
-      <c r="Z15" s="18"/>
-      <c r="AA15" s="18"/>
-      <c r="AB15" s="18"/>
-      <c r="AC15" s="18"/>
-      <c r="AD15" s="18"/>
-      <c r="AE15" s="18"/>
-      <c r="AF15" s="18"/>
-      <c r="AG15" s="18"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="17"/>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="17"/>
+      <c r="AE15" s="17"/>
+      <c r="AF15" s="17"/>
+      <c r="AG15" s="17"/>
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
       <c r="AJ15" s="6"/>
     </row>
     <row r="16" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="23" t="s">
-        <v>134</v>
+      <c r="B16" s="22" t="s">
+        <v>131</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="18" t="s">
-        <v>113</v>
+      <c r="E16" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="19"/>
-      <c r="X16" s="19"/>
-      <c r="Y16" s="19"/>
-      <c r="Z16" s="19"/>
-      <c r="AA16" s="19"/>
-      <c r="AB16" s="19"/>
-      <c r="AC16" s="19"/>
-      <c r="AD16" s="19"/>
-      <c r="AE16" s="19"/>
-      <c r="AF16" s="19"/>
-      <c r="AG16" s="19"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="18"/>
+      <c r="Y16" s="18"/>
+      <c r="Z16" s="18"/>
+      <c r="AA16" s="18"/>
+      <c r="AB16" s="18"/>
+      <c r="AC16" s="18"/>
+      <c r="AD16" s="18"/>
+      <c r="AE16" s="18"/>
+      <c r="AF16" s="18"/>
+      <c r="AG16" s="18"/>
       <c r="AH16" s="7"/>
       <c r="AI16" s="6"/>
       <c r="AJ16" s="6"/>
     </row>
     <row r="17" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="23" t="s">
-        <v>134</v>
+      <c r="B17" s="22" t="s">
+        <v>131</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="18" t="s">
-        <v>113</v>
+      <c r="E17" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
@@ -2891,45 +2891,45 @@
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
-      <c r="W17" s="18"/>
-      <c r="X17" s="18"/>
-      <c r="Y17" s="18"/>
-      <c r="Z17" s="18"/>
-      <c r="AA17" s="18"/>
-      <c r="AB17" s="18"/>
-      <c r="AC17" s="18"/>
-      <c r="AD17" s="18"/>
-      <c r="AE17" s="18"/>
-      <c r="AF17" s="18"/>
-      <c r="AG17" s="18"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="17"/>
+      <c r="Y17" s="17"/>
+      <c r="Z17" s="17"/>
+      <c r="AA17" s="17"/>
+      <c r="AB17" s="17"/>
+      <c r="AC17" s="17"/>
+      <c r="AD17" s="17"/>
+      <c r="AE17" s="17"/>
+      <c r="AF17" s="17"/>
+      <c r="AG17" s="17"/>
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
       <c r="AJ17" s="6"/>
     </row>
     <row r="18" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="C18" s="18"/>
+      <c r="B18" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="17"/>
       <c r="D18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="18" t="s">
-        <v>113</v>
+      <c r="E18" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -2937,45 +2937,45 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
-      <c r="X18" s="18"/>
-      <c r="Y18" s="18"/>
-      <c r="Z18" s="18"/>
-      <c r="AA18" s="18"/>
-      <c r="AB18" s="18"/>
-      <c r="AC18" s="18"/>
-      <c r="AD18" s="18"/>
-      <c r="AE18" s="18"/>
-      <c r="AF18" s="18"/>
-      <c r="AG18" s="18"/>
-      <c r="AH18" s="18"/>
-      <c r="AI18" s="18"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="17"/>
+      <c r="AA18" s="17"/>
+      <c r="AB18" s="17"/>
+      <c r="AC18" s="17"/>
+      <c r="AD18" s="17"/>
+      <c r="AE18" s="17"/>
+      <c r="AF18" s="17"/>
+      <c r="AG18" s="17"/>
+      <c r="AH18" s="17"/>
+      <c r="AI18" s="17"/>
       <c r="AJ18" s="6"/>
     </row>
     <row r="19" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="C19" s="18"/>
+      <c r="B19" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="17"/>
       <c r="D19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>113</v>
+      <c r="E19" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -2983,34 +2983,34 @@
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="18"/>
-      <c r="V19" s="18"/>
-      <c r="W19" s="18"/>
-      <c r="X19" s="18"/>
-      <c r="Y19" s="18"/>
-      <c r="Z19" s="18"/>
-      <c r="AA19" s="18"/>
-      <c r="AB19" s="18"/>
-      <c r="AC19" s="18"/>
-      <c r="AD19" s="18"/>
-      <c r="AE19" s="18"/>
-      <c r="AF19" s="18"/>
-      <c r="AG19" s="18"/>
-      <c r="AH19" s="18"/>
-      <c r="AI19" s="18"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="17"/>
+      <c r="AA19" s="17"/>
+      <c r="AB19" s="17"/>
+      <c r="AC19" s="17"/>
+      <c r="AD19" s="17"/>
+      <c r="AE19" s="17"/>
+      <c r="AF19" s="17"/>
+      <c r="AG19" s="17"/>
+      <c r="AH19" s="17"/>
+      <c r="AI19" s="17"/>
       <c r="AJ19" s="6"/>
     </row>
     <row r="20" spans="1:36" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="6"/>
@@ -3050,7 +3050,7 @@
       <c r="AJ20" s="6"/>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -3061,28 +3061,28 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
-      <c r="S21" s="19"/>
-      <c r="T21" s="19"/>
-      <c r="U21" s="19"/>
-      <c r="V21" s="19"/>
-      <c r="W21" s="19"/>
-      <c r="X21" s="19"/>
-      <c r="Y21" s="19"/>
-      <c r="Z21" s="19"/>
-      <c r="AA21" s="19"/>
-      <c r="AB21" s="19"/>
-      <c r="AC21" s="19"/>
-      <c r="AD21" s="19"/>
-      <c r="AE21" s="19"/>
-      <c r="AF21" s="19"/>
-      <c r="AG21" s="19"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="18"/>
+      <c r="V21" s="18"/>
+      <c r="W21" s="18"/>
+      <c r="X21" s="18"/>
+      <c r="Y21" s="18"/>
+      <c r="Z21" s="18"/>
+      <c r="AA21" s="18"/>
+      <c r="AB21" s="18"/>
+      <c r="AC21" s="18"/>
+      <c r="AD21" s="18"/>
+      <c r="AE21" s="18"/>
+      <c r="AF21" s="18"/>
+      <c r="AG21" s="18"/>
       <c r="AH21" s="7"/>
       <c r="AI21" s="6"/>
       <c r="AJ21" s="6"/>
@@ -3099,288 +3099,298 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BD2F75-093A-4CCC-AFDF-54FE23EAD35D}">
-  <dimension ref="A1:AF21"/>
+  <dimension ref="A1:AJ21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" style="1" customWidth="1"/>
-    <col min="20" max="21" width="19.140625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="16.5703125" style="1" customWidth="1"/>
-    <col min="23" max="24" width="16.7109375" style="1" customWidth="1"/>
-    <col min="25" max="25" width="17.140625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="16.42578125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="16.140625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="21.140625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="30.85546875" style="1" customWidth="1"/>
-    <col min="30" max="30" width="17" style="1" customWidth="1"/>
-    <col min="31" max="31" width="15.7109375" style="1" customWidth="1"/>
-    <col min="32" max="32" width="14.42578125" style="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8.140625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="28" style="12" customWidth="1"/>
+    <col min="3" max="3" width="16" style="12" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="12" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="12" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="12" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="12" customWidth="1"/>
+    <col min="14" max="14" width="20" style="12" customWidth="1"/>
+    <col min="15" max="16" width="17.42578125" style="12" customWidth="1"/>
+    <col min="17" max="17" width="24" style="12" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" style="12" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" style="12" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" style="12" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" style="12" customWidth="1"/>
+    <col min="22" max="22" width="5.7109375" style="12" customWidth="1"/>
+    <col min="23" max="23" width="8" style="12" customWidth="1"/>
+    <col min="24" max="24" width="13" style="12" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" style="12" customWidth="1"/>
+    <col min="26" max="26" width="23.28515625" style="12" customWidth="1"/>
+    <col min="27" max="28" width="16.7109375" style="12" customWidth="1"/>
+    <col min="29" max="29" width="17.140625" style="12" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="12" customWidth="1"/>
+    <col min="31" max="31" width="16.140625" style="12" customWidth="1"/>
+    <col min="32" max="32" width="21.140625" style="12" customWidth="1"/>
+    <col min="33" max="33" width="30.85546875" style="12" customWidth="1"/>
+    <col min="34" max="34" width="17" style="12" customWidth="1"/>
+    <col min="35" max="35" width="15.7109375" style="12" customWidth="1"/>
+    <col min="36" max="36" width="14.42578125" style="12" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-    </row>
-    <row r="2" spans="1:32" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-    </row>
-    <row r="3" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="1" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+    </row>
+    <row r="2" spans="1:36" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13"/>
+    </row>
+    <row r="3" spans="1:36" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="11" t="s">
+      <c r="F3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="S3" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q3" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="R3" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="S3" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="T3" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="U3" s="11" t="s">
+      <c r="T3" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="W3" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="X3" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="11"/>
-      <c r="AC3" s="11"/>
-      <c r="AD3" s="11"/>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="11"/>
-    </row>
-    <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="14"/>
+      <c r="AF3" s="14"/>
+      <c r="AG3" s="14"/>
+      <c r="AH3" s="14"/>
+      <c r="AI3" s="14"/>
+      <c r="AJ3" s="14"/>
+    </row>
+    <row r="4" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="B4" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>25</v>
+        <v>122</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="H4" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="L4" s="6" t="s">
-        <v>71</v>
+        <v>143</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>70</v>
+        <v>142</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="R4" s="6" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
+      <c r="X4" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>108</v>
+      </c>
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
       <c r="AE4" s="6"/>
       <c r="AF4" s="6"/>
-    </row>
-    <row r="5" spans="1:32" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+    </row>
+    <row r="5" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="B5" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>72</v>
-      </c>
       <c r="L5" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>89</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="M5" s="17"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
       <c r="T5" s="6"/>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
@@ -3394,52 +3404,44 @@
       <c r="AD5" s="6"/>
       <c r="AE5" s="6"/>
       <c r="AF5" s="6"/>
-    </row>
-    <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
+    </row>
+    <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="B6" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="10" t="s">
-        <v>25</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>73</v>
-      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
+      <c r="M6" s="17"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
-      <c r="R6" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
       <c r="W6" s="7"/>
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
@@ -3447,69 +3449,47 @@
       <c r="AA6" s="7"/>
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
-      <c r="AD6" s="6"/>
-      <c r="AE6" s="6"/>
-      <c r="AF6" s="6"/>
-    </row>
-    <row r="7" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="6"/>
+    </row>
+    <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="B7" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="10" t="s">
-        <v>25</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>85</v>
-      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
-      <c r="R7" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="S7" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="T7" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="U7" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="V7" s="7"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
       <c r="Y7" s="7"/>
@@ -3517,65 +3497,45 @@
       <c r="AA7" s="7"/>
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
-      <c r="AD7" s="6"/>
-      <c r="AE7" s="6"/>
-      <c r="AF7" s="6"/>
-    </row>
-    <row r="8" spans="1:32" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="6"/>
+      <c r="AJ7" s="6"/>
+    </row>
+    <row r="8" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="B8" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="10" t="s">
-        <v>25</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="S8" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="T8" s="7" t="s">
-        <v>91</v>
-      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
@@ -3588,42 +3548,44 @@
       <c r="AD8" s="6"/>
       <c r="AE8" s="6"/>
       <c r="AF8" s="6"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="6"/>
+    </row>
+    <row r="9" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="B9" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="10" t="s">
-        <v>25</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+      <c r="M9" s="17"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
       <c r="W9" s="7"/>
       <c r="X9" s="7"/>
       <c r="Y9" s="7"/>
@@ -3631,22 +3593,36 @@
       <c r="AA9" s="7"/>
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
-      <c r="AD9" s="6"/>
-      <c r="AE9" s="6"/>
-      <c r="AF9" s="6"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="6"/>
+      <c r="AJ9" s="6"/>
+    </row>
+    <row r="10" spans="1:36" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="22" t="s">
+        <v>119</v>
+      </c>
       <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="D10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>127</v>
+      </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="I10" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -3656,10 +3632,10 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
       <c r="W10" s="7"/>
       <c r="X10" s="7"/>
       <c r="Y10" s="7"/>
@@ -3668,335 +3644,457 @@
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
-      <c r="AE10" s="6"/>
-      <c r="AF10" s="6"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="7"/>
+      <c r="AH10" s="7"/>
+      <c r="AI10" s="6"/>
+      <c r="AJ10" s="6"/>
+    </row>
+    <row r="11" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="22" t="s">
+        <v>119</v>
+      </c>
       <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="5"/>
+      <c r="I11" s="6" t="s">
+        <v>126</v>
+      </c>
       <c r="J11" s="6"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
-      <c r="AA11" s="5"/>
-      <c r="AB11" s="5"/>
-      <c r="AC11" s="5"/>
-      <c r="AD11" s="6"/>
-      <c r="AE11" s="6"/>
-      <c r="AF11" s="6"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
+      <c r="AA11" s="17"/>
+      <c r="AB11" s="17"/>
+      <c r="AC11" s="17"/>
+      <c r="AD11" s="17"/>
+      <c r="AE11" s="17"/>
+      <c r="AF11" s="17"/>
+      <c r="AG11" s="17"/>
+      <c r="AH11" s="6"/>
+      <c r="AI11" s="6"/>
+      <c r="AJ11" s="6"/>
+    </row>
+    <row r="12" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="22" t="s">
+        <v>119</v>
+      </c>
       <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="D12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>129</v>
+      </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="5"/>
-      <c r="Y12" s="5"/>
-      <c r="Z12" s="5"/>
-      <c r="AA12" s="5"/>
-      <c r="AB12" s="5"/>
-      <c r="AC12" s="5"/>
-      <c r="AD12" s="6"/>
-      <c r="AE12" s="6"/>
-      <c r="AF12" s="6"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="I12" s="6"/>
+      <c r="J12" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="17"/>
+      <c r="AA12" s="17"/>
+      <c r="AB12" s="17"/>
+      <c r="AC12" s="17"/>
+      <c r="AD12" s="17"/>
+      <c r="AE12" s="17"/>
+      <c r="AF12" s="17"/>
+      <c r="AG12" s="17"/>
+      <c r="AH12" s="6"/>
+      <c r="AI12" s="6"/>
+      <c r="AJ12" s="6"/>
+    </row>
+    <row r="13" spans="1:36" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="B13" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>110</v>
+      </c>
       <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
-      <c r="X13" s="5"/>
-      <c r="Y13" s="5"/>
-      <c r="Z13" s="5"/>
-      <c r="AA13" s="5"/>
-      <c r="AB13" s="5"/>
-      <c r="AC13" s="5"/>
-      <c r="AD13" s="6"/>
-      <c r="AE13" s="6"/>
-      <c r="AF13" s="6"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="G13" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="17"/>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17"/>
+      <c r="AA13" s="17"/>
+      <c r="AB13" s="17"/>
+      <c r="AC13" s="17"/>
+      <c r="AD13" s="17"/>
+      <c r="AE13" s="17"/>
+      <c r="AF13" s="17"/>
+      <c r="AG13" s="17"/>
+      <c r="AH13" s="6"/>
+      <c r="AI13" s="6"/>
+      <c r="AJ13" s="6"/>
+    </row>
+    <row r="14" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="22" t="s">
+        <v>131</v>
+      </c>
       <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="D14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>122</v>
+      </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="5"/>
-      <c r="W14" s="5"/>
-      <c r="X14" s="5"/>
-      <c r="Y14" s="5"/>
-      <c r="Z14" s="5"/>
-      <c r="AA14" s="5"/>
-      <c r="AB14" s="5"/>
-      <c r="AC14" s="5"/>
-      <c r="AD14" s="6"/>
-      <c r="AE14" s="6"/>
-      <c r="AF14" s="6"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="17"/>
+      <c r="AA14" s="17"/>
+      <c r="AB14" s="17"/>
+      <c r="AC14" s="17"/>
+      <c r="AD14" s="17"/>
+      <c r="AE14" s="17"/>
+      <c r="AF14" s="17"/>
+      <c r="AG14" s="17"/>
+      <c r="AH14" s="6"/>
+      <c r="AI14" s="6"/>
+      <c r="AJ14" s="6"/>
+    </row>
+    <row r="15" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="22" t="s">
+        <v>131</v>
+      </c>
       <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="D15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>122</v>
+      </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="5"/>
-      <c r="Z15" s="5"/>
-      <c r="AA15" s="5"/>
-      <c r="AB15" s="5"/>
-      <c r="AC15" s="5"/>
-      <c r="AD15" s="6"/>
-      <c r="AE15" s="6"/>
-      <c r="AF15" s="6"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="17"/>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="17"/>
+      <c r="AE15" s="17"/>
+      <c r="AF15" s="17"/>
+      <c r="AG15" s="17"/>
+      <c r="AH15" s="6"/>
+      <c r="AI15" s="6"/>
+      <c r="AJ15" s="6"/>
+    </row>
+    <row r="16" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="22" t="s">
+        <v>131</v>
+      </c>
       <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="D16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>139</v>
+      </c>
       <c r="H16" s="6"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="8"/>
-      <c r="Z16" s="8"/>
-      <c r="AA16" s="8"/>
-      <c r="AB16" s="8"/>
-      <c r="AC16" s="8"/>
-      <c r="AD16" s="7"/>
-      <c r="AE16" s="6"/>
-      <c r="AF16" s="6"/>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="18"/>
+      <c r="Y16" s="18"/>
+      <c r="Z16" s="18"/>
+      <c r="AA16" s="18"/>
+      <c r="AB16" s="18"/>
+      <c r="AC16" s="18"/>
+      <c r="AD16" s="18"/>
+      <c r="AE16" s="18"/>
+      <c r="AF16" s="18"/>
+      <c r="AG16" s="18"/>
+      <c r="AH16" s="7"/>
+      <c r="AI16" s="6"/>
+      <c r="AJ16" s="6"/>
+    </row>
+    <row r="17" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="22" t="s">
+        <v>131</v>
+      </c>
       <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="D17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>110</v>
+      </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5"/>
-      <c r="X17" s="5"/>
-      <c r="Y17" s="5"/>
-      <c r="Z17" s="5"/>
-      <c r="AA17" s="5"/>
-      <c r="AB17" s="5"/>
-      <c r="AC17" s="5"/>
-      <c r="AD17" s="6"/>
-      <c r="AE17" s="6"/>
-      <c r="AF17" s="6"/>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="17"/>
+      <c r="Y17" s="17"/>
+      <c r="Z17" s="17"/>
+      <c r="AA17" s="17"/>
+      <c r="AB17" s="17"/>
+      <c r="AC17" s="17"/>
+      <c r="AD17" s="17"/>
+      <c r="AE17" s="17"/>
+      <c r="AF17" s="17"/>
+      <c r="AG17" s="17"/>
+      <c r="AH17" s="6"/>
+      <c r="AI17" s="6"/>
+      <c r="AJ17" s="6"/>
+    </row>
+    <row r="18" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
+      <c r="B18" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>110</v>
+      </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
-      <c r="V18" s="5"/>
-      <c r="W18" s="5"/>
-      <c r="X18" s="5"/>
-      <c r="Y18" s="5"/>
-      <c r="Z18" s="5"/>
-      <c r="AA18" s="5"/>
-      <c r="AB18" s="5"/>
-      <c r="AC18" s="5"/>
-      <c r="AD18" s="5"/>
-      <c r="AE18" s="5"/>
-      <c r="AF18" s="6"/>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="17"/>
+      <c r="AA18" s="17"/>
+      <c r="AB18" s="17"/>
+      <c r="AC18" s="17"/>
+      <c r="AD18" s="17"/>
+      <c r="AE18" s="17"/>
+      <c r="AF18" s="17"/>
+      <c r="AG18" s="17"/>
+      <c r="AH18" s="17"/>
+      <c r="AI18" s="17"/>
+      <c r="AJ18" s="6"/>
+    </row>
+    <row r="19" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
+      <c r="B19" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>110</v>
+      </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
-      <c r="V19" s="5"/>
-      <c r="W19" s="5"/>
-      <c r="X19" s="5"/>
-      <c r="Y19" s="5"/>
-      <c r="Z19" s="5"/>
-      <c r="AA19" s="5"/>
-      <c r="AB19" s="5"/>
-      <c r="AC19" s="5"/>
-      <c r="AD19" s="5"/>
-      <c r="AE19" s="5"/>
-      <c r="AF19" s="6"/>
-    </row>
-    <row r="20" spans="1:32" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="17"/>
+      <c r="AA19" s="17"/>
+      <c r="AB19" s="17"/>
+      <c r="AC19" s="17"/>
+      <c r="AD19" s="17"/>
+      <c r="AE19" s="17"/>
+      <c r="AF19" s="17"/>
+      <c r="AG19" s="17"/>
+      <c r="AH19" s="17"/>
+      <c r="AI19" s="17"/>
+      <c r="AJ19" s="6"/>
+    </row>
+    <row r="20" spans="1:36" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="6"/>
@@ -4030,9 +4128,13 @@
       <c r="AD20" s="6"/>
       <c r="AE20" s="6"/>
       <c r="AF20" s="6"/>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="AG20" s="6"/>
+      <c r="AH20" s="6"/>
+      <c r="AI20" s="6"/>
+      <c r="AJ20" s="6"/>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A21" s="16"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -4040,39 +4142,39 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="8"/>
-      <c r="W21" s="8"/>
-      <c r="X21" s="8"/>
-      <c r="Y21" s="8"/>
-      <c r="Z21" s="8"/>
-      <c r="AA21" s="8"/>
-      <c r="AB21" s="8"/>
-      <c r="AC21" s="8"/>
-      <c r="AD21" s="7"/>
-      <c r="AE21" s="6"/>
-      <c r="AF21" s="6"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="18"/>
+      <c r="V21" s="18"/>
+      <c r="W21" s="18"/>
+      <c r="X21" s="18"/>
+      <c r="Y21" s="18"/>
+      <c r="Z21" s="18"/>
+      <c r="AA21" s="18"/>
+      <c r="AB21" s="18"/>
+      <c r="AC21" s="18"/>
+      <c r="AD21" s="18"/>
+      <c r="AE21" s="18"/>
+      <c r="AF21" s="18"/>
+      <c r="AG21" s="18"/>
+      <c r="AH21" s="7"/>
+      <c r="AI21" s="6"/>
+      <c r="AJ21" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A1:AJ1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" xr:uid="{36A369D6-E91B-49AE-8B24-4F98FC641AA4}"/>
-    <hyperlink ref="C6" r:id="rId2" xr:uid="{0703A915-9653-412D-B56E-A64DD871DA0F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4121,131 +4223,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="29"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
     </row>
     <row r="2" spans="1:32" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
     </row>
     <row r="3" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="S3" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="T3" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="U3" s="12" t="s">
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="X3" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y3" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z3" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA3" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB3" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="V3" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="W3" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="X3" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y3" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z3" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA3" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB3" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="AC3" s="12"/>
-      <c r="AD3" s="12"/>
-      <c r="AE3" s="12"/>
-      <c r="AF3" s="12"/>
+      <c r="AC3" s="11"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="11"/>
     </row>
     <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -4299,12 +4401,12 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
       <c r="V4" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="W4" s="7" t="s">
         <v>39</v>
@@ -4313,10 +4415,10 @@
         <v>39</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
@@ -4375,7 +4477,7 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
       <c r="S5" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="T5" s="6"/>
       <c r="U5" s="6"/>
@@ -4428,7 +4530,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
       <c r="S6" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
@@ -4472,33 +4574,33 @@
         <v>58</v>
       </c>
       <c r="K7" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>76</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
       <c r="S7" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="V7" s="7" t="s">
         <v>39</v>
@@ -4546,30 +4648,30 @@
         <v>58</v>
       </c>
       <c r="K8" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="M8" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>76</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
       <c r="S8" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="U8" s="6"/>
       <c r="W8" s="6"/>

</xml_diff>

<commit_message>
Checking filtered page content
</commit_message>
<xml_diff>
--- a/src/test/test_data/gigatron.xlsx
+++ b/src/test/test_data/gigatron.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\gigatron\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C4FE60-0C90-4C12-ABE3-89F30DEE2CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1231B4E2-C6E3-4ABB-9863-EE6E2DDBD3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="checkout" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="152">
   <si>
     <t>tc_id</t>
   </si>
@@ -472,6 +473,18 @@
   </si>
   <si>
     <t>value2</t>
+  </si>
+  <si>
+    <t>filter3</t>
+  </si>
+  <si>
+    <t>value3</t>
+  </si>
+  <si>
+    <t>Tip procesora</t>
+  </si>
+  <si>
+    <t>Intel Core i9</t>
   </si>
 </sst>
 </file>
@@ -3102,7 +3115,7 @@
   <dimension ref="A1:AJ21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3213,7 +3226,7 @@
         <v>145</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="J3" s="14" t="s">
         <v>102</v>
@@ -3228,7 +3241,7 @@
         <v>147</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="O3" s="14" t="s">
         <v>48</v>
@@ -3296,7 +3309,9 @@
       <c r="H4" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="I4" s="6"/>
+      <c r="I4" s="6" t="s">
+        <v>150</v>
+      </c>
       <c r="J4" s="10"/>
       <c r="K4" s="6" t="s">
         <v>36</v>
@@ -3308,7 +3323,7 @@
         <v>142</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>41</v>
+        <v>151</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>42</v>

</xml_diff>